<commit_message>
se agrega columna remesa
</commit_message>
<xml_diff>
--- a/assets/informe_polar.xlsx
+++ b/assets/informe_polar.xlsx
@@ -183,154 +183,384 @@
     <author>Funcionario MCT</author>
   </authors>
   <commentList>
-    <comment ref="K10" authorId="0" shapeId="0">
+    <comment ref="J9" authorId="0" shapeId="0">
+      <text>
+        <t>h</t>
+      </text>
+    </comment>
+    <comment ref="K9" authorId="0" shapeId="0">
+      <text>
+        <t>r</t>
+      </text>
+    </comment>
+    <comment ref="L9" authorId="0" shapeId="0">
+      <text>
+        <t>f</t>
+      </text>
+    </comment>
+    <comment ref="M9" authorId="0" shapeId="0">
+      <text>
+        <t>u</t>
+      </text>
+    </comment>
+    <comment ref="N9" authorId="0" shapeId="0">
+      <text>
+        <t>j</t>
+      </text>
+    </comment>
+    <comment ref="O9" authorId="0" shapeId="0">
+      <text>
+        <t>y</t>
+      </text>
+    </comment>
+    <comment ref="P9" authorId="0" shapeId="0">
+      <text>
+        <t>u</t>
+      </text>
+    </comment>
+    <comment ref="Q9" authorId="0" shapeId="0">
+      <text>
+        <t>r</t>
+      </text>
+    </comment>
+    <comment ref="R9" authorId="0" shapeId="0">
+      <text>
+        <t>k</t>
+      </text>
+    </comment>
+    <comment ref="S9" authorId="0" shapeId="0">
+      <text>
+        <t>k</t>
+      </text>
+    </comment>
+    <comment ref="T9" authorId="0" shapeId="0">
+      <text>
+        <t>g</t>
+      </text>
+    </comment>
+    <comment ref="L10" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="L10" authorId="0" shapeId="0">
+    <comment ref="M10" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="M10" authorId="0" shapeId="0">
+    <comment ref="N10" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="K11" authorId="0" shapeId="0">
+    <comment ref="L11" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="L11" authorId="0" shapeId="0">
+    <comment ref="M11" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="M11" authorId="0" shapeId="0">
+    <comment ref="N11" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="K21" authorId="0" shapeId="0">
+    <comment ref="L19" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">. </t>
+      </text>
+    </comment>
+    <comment ref="R19" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">descargaron en el transcurso de la noche </t>
+      </text>
+    </comment>
+    <comment ref="S19" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">descargaron en el transcurso de la noche </t>
+      </text>
+    </comment>
+    <comment ref="T19" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">retorno al día siguiente día </t>
+      </text>
+    </comment>
+    <comment ref="L21" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="L21" authorId="0" shapeId="0">
+    <comment ref="M21" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="M21" authorId="0" shapeId="0">
+    <comment ref="N21" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="K29" authorId="0" shapeId="0">
+    <comment ref="L29" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="L29" authorId="0" shapeId="0">
+    <comment ref="M29" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="M29" authorId="0" shapeId="0">
+    <comment ref="N29" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="K30" authorId="0" shapeId="0">
+    <comment ref="L30" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="L30" authorId="0" shapeId="0">
+    <comment ref="M30" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="M30" authorId="0" shapeId="0">
+    <comment ref="N30" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="K31" authorId="0" shapeId="0">
+    <comment ref="L31" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="L31" authorId="0" shapeId="0">
+    <comment ref="M31" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="M31" authorId="0" shapeId="0">
+    <comment ref="N31" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="K32" authorId="0" shapeId="0">
+    <comment ref="L32" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="L32" authorId="0" shapeId="0">
+    <comment ref="M32" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="M32" authorId="0" shapeId="0">
+    <comment ref="N32" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">S/N </t>
       </text>
     </comment>
-    <comment ref="K35" authorId="0" shapeId="0">
+    <comment ref="L34" authorId="0" shapeId="0">
       <text>
         <t>ok</t>
       </text>
     </comment>
-    <comment ref="L35" authorId="0" shapeId="0">
+    <comment ref="M34" authorId="0" shapeId="0">
       <text>
         <t>ok</t>
       </text>
     </comment>
-    <comment ref="M35" authorId="0" shapeId="0">
+    <comment ref="N34" authorId="0" shapeId="0">
       <text>
         <t>ok</t>
       </text>
     </comment>
-    <comment ref="K38" authorId="0" shapeId="0">
+    <comment ref="L37" authorId="0" shapeId="0">
       <text>
         <t>ok</t>
       </text>
     </comment>
-    <comment ref="L38" authorId="0" shapeId="0">
+    <comment ref="M37" authorId="0" shapeId="0">
       <text>
         <t>ok</t>
       </text>
     </comment>
-    <comment ref="M38" authorId="0" shapeId="0">
+    <comment ref="N37" authorId="0" shapeId="0">
       <text>
         <t>ok</t>
       </text>
     </comment>
-    <comment ref="K43" authorId="0" shapeId="0">
+    <comment ref="L42" authorId="0" shapeId="0">
       <text>
         <t>ok</t>
       </text>
     </comment>
-    <comment ref="L43" authorId="0" shapeId="0">
+    <comment ref="M42" authorId="0" shapeId="0">
       <text>
         <t>ok</t>
       </text>
     </comment>
-    <comment ref="M43" authorId="0" shapeId="0">
+    <comment ref="N42" authorId="0" shapeId="0">
       <text>
         <t>ok</t>
+      </text>
+    </comment>
+    <comment ref="J45" authorId="0" shapeId="0">
+      <text>
+        <t>u</t>
+      </text>
+    </comment>
+    <comment ref="K45" authorId="0" shapeId="0">
+      <text>
+        <t>h</t>
+      </text>
+    </comment>
+    <comment ref="L45" authorId="0" shapeId="0">
+      <text>
+        <t>f</t>
+      </text>
+    </comment>
+    <comment ref="M45" authorId="0" shapeId="0">
+      <text>
+        <t>u</t>
+      </text>
+    </comment>
+    <comment ref="N45" authorId="0" shapeId="0">
+      <text>
+        <t>f</t>
+      </text>
+    </comment>
+    <comment ref="O45" authorId="0" shapeId="0">
+      <text>
+        <t>h</t>
+      </text>
+    </comment>
+    <comment ref="L46" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">S/N </t>
+      </text>
+    </comment>
+    <comment ref="M46" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">S/N </t>
+      </text>
+    </comment>
+    <comment ref="N46" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">S/N </t>
+      </text>
+    </comment>
+    <comment ref="Q46" authorId="0" shapeId="0">
+      <text>
+        <t>el vehículo lo descargaron en el transcurso del día 3/02/2022</t>
+      </text>
+    </comment>
+    <comment ref="R46" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">el vehículo lo descargaron en el transcurso del día </t>
+      </text>
+    </comment>
+    <comment ref="J51" authorId="0" shapeId="0">
+      <text>
+        <t>u</t>
+      </text>
+    </comment>
+    <comment ref="K51" authorId="0" shapeId="0">
+      <text>
+        <t>r</t>
+      </text>
+    </comment>
+    <comment ref="L51" authorId="0" shapeId="0">
+      <text>
+        <t>r</t>
+      </text>
+    </comment>
+    <comment ref="M51" authorId="0" shapeId="0">
+      <text>
+        <t>t</t>
+      </text>
+    </comment>
+    <comment ref="N51" authorId="0" shapeId="0">
+      <text>
+        <t>g</t>
+      </text>
+    </comment>
+    <comment ref="O51" authorId="0" shapeId="0">
+      <text>
+        <t>j</t>
+      </text>
+    </comment>
+    <comment ref="P51" authorId="0" shapeId="0">
+      <text>
+        <t>j</t>
+      </text>
+    </comment>
+    <comment ref="Q51" authorId="0" shapeId="0">
+      <text>
+        <t>r</t>
+      </text>
+    </comment>
+    <comment ref="R51" authorId="0" shapeId="0">
+      <text>
+        <t>g</t>
+      </text>
+    </comment>
+    <comment ref="S51" authorId="0" shapeId="0">
+      <text>
+        <t>t</t>
+      </text>
+    </comment>
+    <comment ref="T51" authorId="0" shapeId="0">
+      <text>
+        <t>f</t>
+      </text>
+    </comment>
+    <comment ref="L54" authorId="0" shapeId="0">
+      <text>
+        <t>ok</t>
+      </text>
+    </comment>
+    <comment ref="M54" authorId="0" shapeId="0">
+      <text>
+        <t>ok</t>
+      </text>
+    </comment>
+    <comment ref="N54" authorId="0" shapeId="0">
+      <text>
+        <t>ok</t>
+      </text>
+    </comment>
+    <comment ref="L56" authorId="0" shapeId="0">
+      <text>
+        <t>S/N</t>
+      </text>
+    </comment>
+    <comment ref="M56" authorId="0" shapeId="0">
+      <text>
+        <t>S/N</t>
+      </text>
+    </comment>
+    <comment ref="N56" authorId="0" shapeId="0">
+      <text>
+        <t>S/N</t>
+      </text>
+    </comment>
+    <comment ref="L59" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">S/N </t>
+      </text>
+    </comment>
+    <comment ref="M59" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">S/N </t>
+      </text>
+    </comment>
+    <comment ref="N59" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">S/N </t>
       </text>
     </comment>
   </commentList>
@@ -656,7 +886,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z45"/>
+  <dimension ref="A1:AA61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -671,25 +901,26 @@
     <col width="33" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="8" customWidth="1" min="8" max="8"/>
-    <col width="21" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
     <col width="21" customWidth="1" min="10" max="10"/>
     <col width="21" customWidth="1" min="11" max="11"/>
     <col width="21" customWidth="1" min="12" max="12"/>
     <col width="21" customWidth="1" min="13" max="13"/>
     <col width="21" customWidth="1" min="14" max="14"/>
     <col width="21" customWidth="1" min="15" max="15"/>
-    <col width="22" customWidth="1" min="16" max="16"/>
-    <col width="21" customWidth="1" min="17" max="17"/>
+    <col width="21" customWidth="1" min="16" max="16"/>
+    <col width="22" customWidth="1" min="17" max="17"/>
     <col width="21" customWidth="1" min="18" max="18"/>
-    <col width="35" customWidth="1" min="19" max="19"/>
-    <col width="23" customWidth="1" min="20" max="20"/>
+    <col width="21" customWidth="1" min="19" max="19"/>
+    <col width="35" customWidth="1" min="20" max="20"/>
     <col width="23" customWidth="1" min="21" max="21"/>
     <col width="23" customWidth="1" min="22" max="22"/>
     <col width="23" customWidth="1" min="23" max="23"/>
-    <col width="28" customWidth="1" min="24" max="24"/>
-    <col width="22" customWidth="1" min="25" max="25"/>
-    <col width="22" customWidth="1" min="26" max="26"/>
+    <col width="23" customWidth="1" min="24" max="24"/>
+    <col width="28" customWidth="1" min="25" max="25"/>
+    <col width="23" customWidth="1" min="26" max="26"/>
+    <col width="22" customWidth="1" min="27" max="27"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -719,6 +950,7 @@
       <c r="X1" s="5" t="n"/>
       <c r="Y1" s="5" t="n"/>
       <c r="Z1" s="5" t="n"/>
+      <c r="AA1" s="5" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="5" t="n"/>
@@ -747,6 +979,7 @@
       <c r="X2" s="5" t="n"/>
       <c r="Y2" s="5" t="n"/>
       <c r="Z2" s="5" t="n"/>
+      <c r="AA2" s="5" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="n"/>
@@ -775,6 +1008,7 @@
       <c r="X3" s="5" t="n"/>
       <c r="Y3" s="5" t="n"/>
       <c r="Z3" s="5" t="n"/>
+      <c r="AA3" s="5" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="5" t="n"/>
@@ -803,6 +1037,7 @@
       <c r="X4" s="5" t="n"/>
       <c r="Y4" s="5" t="n"/>
       <c r="Z4" s="5" t="n"/>
+      <c r="AA4" s="5" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="n"/>
@@ -831,6 +1066,7 @@
       <c r="X5" s="5" t="n"/>
       <c r="Y5" s="5" t="n"/>
       <c r="Z5" s="5" t="n"/>
+      <c r="AA5" s="5" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="n"/>
@@ -866,95 +1102,100 @@
       </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
+          <t>REMESA</t>
+        </is>
+      </c>
+      <c r="I6" s="7" t="inlineStr">
+        <is>
           <t>PLACA</t>
         </is>
       </c>
-      <c r="I6" s="7" t="inlineStr">
+      <c r="J6" s="7" t="inlineStr">
         <is>
           <t>LLEGADA A PLANTA</t>
         </is>
       </c>
-      <c r="J6" s="7" t="inlineStr">
+      <c r="K6" s="7" t="inlineStr">
         <is>
           <t>INGRESO A PLANTA</t>
         </is>
       </c>
-      <c r="K6" s="7" t="inlineStr">
+      <c r="L6" s="7" t="inlineStr">
         <is>
           <t>INICIO DEL CARGUE</t>
         </is>
       </c>
-      <c r="L6" s="7" t="inlineStr">
+      <c r="M6" s="7" t="inlineStr">
         <is>
           <t>FIN DEL CARGUE</t>
         </is>
       </c>
-      <c r="M6" s="7" t="inlineStr">
+      <c r="N6" s="7" t="inlineStr">
         <is>
           <t>SALIDA DE PLANTA</t>
         </is>
       </c>
-      <c r="N6" s="7" t="inlineStr">
+      <c r="O6" s="7" t="inlineStr">
         <is>
           <t>LLEGADA A DESCARGUE</t>
         </is>
       </c>
-      <c r="O6" s="7" t="inlineStr">
+      <c r="P6" s="7" t="inlineStr">
         <is>
           <t>INGRESO A DESCARGUE</t>
         </is>
       </c>
-      <c r="P6" s="7" t="inlineStr">
+      <c r="Q6" s="7" t="inlineStr">
         <is>
           <t>INICIO DEL DESCARGUE</t>
         </is>
       </c>
-      <c r="Q6" s="7" t="inlineStr">
+      <c r="R6" s="7" t="inlineStr">
         <is>
           <t>FIN DEL DESCARGUE</t>
         </is>
       </c>
-      <c r="R6" s="7" t="inlineStr">
+      <c r="S6" s="7" t="inlineStr">
         <is>
           <t>SALIDA DE DESCARGUE</t>
         </is>
       </c>
-      <c r="S6" s="7" t="inlineStr">
+      <c r="T6" s="7" t="inlineStr">
         <is>
           <t>VEHICULO RETORNADO A PLANTA POLAR</t>
         </is>
       </c>
-      <c r="T6" s="7" t="inlineStr">
+      <c r="U6" s="7" t="inlineStr">
         <is>
           <t>INICIO Round Trip</t>
         </is>
       </c>
-      <c r="U6" s="7" t="inlineStr">
+      <c r="V6" s="7" t="inlineStr">
         <is>
           <t>TIEMPO DE CARGUE</t>
         </is>
       </c>
-      <c r="V6" s="7" t="inlineStr">
+      <c r="W6" s="7" t="inlineStr">
         <is>
           <t>TIEMPO DE SALIDA</t>
         </is>
       </c>
-      <c r="W6" s="7" t="inlineStr">
+      <c r="X6" s="7" t="inlineStr">
         <is>
           <t>TIEMPO EN RUTA</t>
         </is>
       </c>
-      <c r="X6" s="7" t="inlineStr">
+      <c r="Y6" s="7" t="inlineStr">
         <is>
           <t>INICIO LLEGADA A DESCARGAR</t>
         </is>
       </c>
-      <c r="Y6" s="7" t="inlineStr">
+      <c r="Z6" s="7" t="inlineStr">
         <is>
           <t>TIEMPO DE DESCARGUE</t>
         </is>
       </c>
-      <c r="Z6" s="7" t="inlineStr">
+      <c r="AA6" s="7" t="inlineStr">
         <is>
           <t>TIEMPO TOTAL X VIAJE</t>
         </is>
@@ -992,10 +1233,14 @@
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
+          <t>13075-7285</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="inlineStr">
+        <is>
           <t>SNC949</t>
         </is>
       </c>
-      <c r="I7" s="5" t="inlineStr"/>
       <c r="J7" s="5" t="inlineStr"/>
       <c r="K7" s="5" t="inlineStr"/>
       <c r="L7" s="5" t="inlineStr"/>
@@ -1006,13 +1251,14 @@
       <c r="Q7" s="5" t="inlineStr"/>
       <c r="R7" s="5" t="inlineStr"/>
       <c r="S7" s="5" t="inlineStr"/>
-      <c r="T7" s="10" t="inlineStr"/>
+      <c r="T7" s="5" t="inlineStr"/>
       <c r="U7" s="10" t="inlineStr"/>
       <c r="V7" s="10" t="inlineStr"/>
       <c r="W7" s="10" t="inlineStr"/>
       <c r="X7" s="10" t="inlineStr"/>
       <c r="Y7" s="10" t="inlineStr"/>
       <c r="Z7" s="10" t="inlineStr"/>
+      <c r="AA7" s="10" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="8" t="n">
@@ -1046,10 +1292,14 @@
       </c>
       <c r="H8" s="5" t="inlineStr">
         <is>
+          <t>13075-7284</t>
+        </is>
+      </c>
+      <c r="I8" s="5" t="inlineStr">
+        <is>
           <t>SKF030</t>
         </is>
       </c>
-      <c r="I8" s="5" t="inlineStr"/>
       <c r="J8" s="5" t="inlineStr"/>
       <c r="K8" s="5" t="inlineStr"/>
       <c r="L8" s="5" t="inlineStr"/>
@@ -1060,13 +1310,14 @@
       <c r="Q8" s="5" t="inlineStr"/>
       <c r="R8" s="5" t="inlineStr"/>
       <c r="S8" s="5" t="inlineStr"/>
-      <c r="T8" s="10" t="inlineStr"/>
+      <c r="T8" s="5" t="inlineStr"/>
       <c r="U8" s="10" t="inlineStr"/>
       <c r="V8" s="10" t="inlineStr"/>
       <c r="W8" s="10" t="inlineStr"/>
       <c r="X8" s="10" t="inlineStr"/>
       <c r="Y8" s="10" t="inlineStr"/>
       <c r="Z8" s="10" t="inlineStr"/>
+      <c r="AA8" s="10" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="8" t="n">
@@ -1080,7 +1331,7 @@
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
-          <t>GENERADA</t>
+          <t>FINALIZADA</t>
         </is>
       </c>
       <c r="E9" s="5" t="inlineStr">
@@ -1100,27 +1351,68 @@
       </c>
       <c r="H9" s="5" t="inlineStr">
         <is>
+          <t>13075-7281</t>
+        </is>
+      </c>
+      <c r="I9" s="5" t="inlineStr">
+        <is>
           <t>SJQ652</t>
         </is>
       </c>
-      <c r="I9" s="5" t="inlineStr"/>
-      <c r="J9" s="5" t="inlineStr"/>
-      <c r="K9" s="5" t="inlineStr"/>
-      <c r="L9" s="5" t="inlineStr"/>
-      <c r="M9" s="5" t="inlineStr"/>
-      <c r="N9" s="5" t="inlineStr"/>
-      <c r="O9" s="5" t="inlineStr"/>
-      <c r="P9" s="5" t="inlineStr"/>
-      <c r="Q9" s="5" t="inlineStr"/>
-      <c r="R9" s="5" t="inlineStr"/>
-      <c r="S9" s="5" t="inlineStr"/>
-      <c r="T9" s="10" t="inlineStr"/>
-      <c r="U9" s="10" t="inlineStr"/>
-      <c r="V9" s="10" t="inlineStr"/>
-      <c r="W9" s="10" t="inlineStr"/>
-      <c r="X9" s="10" t="inlineStr"/>
-      <c r="Y9" s="10" t="inlineStr"/>
-      <c r="Z9" s="10" t="inlineStr"/>
+      <c r="J9" s="11" t="n">
+        <v>44595.51143518519</v>
+      </c>
+      <c r="K9" s="11" t="n">
+        <v>44595.51366898148</v>
+      </c>
+      <c r="L9" s="11" t="n">
+        <v>44595.51381944444</v>
+      </c>
+      <c r="M9" s="11" t="n">
+        <v>44595.53818287037</v>
+      </c>
+      <c r="N9" s="11" t="n">
+        <v>44595.54</v>
+      </c>
+      <c r="O9" s="11" t="n">
+        <v>44595.57706018518</v>
+      </c>
+      <c r="P9" s="11" t="n">
+        <v>44595.57715277778</v>
+      </c>
+      <c r="Q9" s="11" t="n">
+        <v>44595.61541666667</v>
+      </c>
+      <c r="R9" s="11" t="n">
+        <v>44595.68003472222</v>
+      </c>
+      <c r="S9" s="11" t="n">
+        <v>44595.68013888889</v>
+      </c>
+      <c r="T9" s="11" t="n">
+        <v>44595.71510416667</v>
+      </c>
+      <c r="U9" s="10" t="n">
+        <v>0.002384259259259259</v>
+      </c>
+      <c r="V9" s="10" t="n">
+        <v>0.02436342592592593</v>
+      </c>
+      <c r="W9" s="10" t="n">
+        <v>0.00181712962962963</v>
+      </c>
+      <c r="X9" s="10" t="n">
+        <v>0.03706018518518518</v>
+      </c>
+      <c r="Y9" s="10" t="n">
+        <v>0.03835648148148148</v>
+      </c>
+      <c r="Z9" s="10" t="n">
+        <v>0.06461805555555555</v>
+      </c>
+      <c r="AA9" s="10" t="n">
+        <v>0.2036689814814815</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="n">
@@ -1154,61 +1446,66 @@
       </c>
       <c r="H10" s="5" t="inlineStr">
         <is>
+          <t>13075-7254</t>
+        </is>
+      </c>
+      <c r="I10" s="5" t="inlineStr">
+        <is>
           <t>SMK294</t>
         </is>
       </c>
-      <c r="I10" s="11" t="n">
-        <v>44593.32498842593</v>
-      </c>
       <c r="J10" s="11" t="n">
-        <v>44593.33887731482</v>
+        <v>44593.11665509259</v>
       </c>
       <c r="K10" s="11" t="n">
-        <v>44593.33908564815</v>
+        <v>44593.13054398148</v>
       </c>
       <c r="L10" s="11" t="n">
-        <v>44593.36140046296</v>
+        <v>44593.13075231481</v>
       </c>
       <c r="M10" s="11" t="n">
-        <v>44593.36581018518</v>
+        <v>44593.15306712963</v>
       </c>
       <c r="N10" s="11" t="n">
-        <v>44593.40119212963</v>
+        <v>44593.15747685185</v>
       </c>
       <c r="O10" s="11" t="n">
-        <v>44593.40277777778</v>
+        <v>44593.1928587963</v>
       </c>
       <c r="P10" s="11" t="n">
-        <v>44593.40966435185</v>
+        <v>44593.19444444445</v>
       </c>
       <c r="Q10" s="11" t="n">
-        <v>44593.50826388889</v>
+        <v>44593.20133101852</v>
       </c>
       <c r="R10" s="11" t="n">
-        <v>44593.50831018519</v>
+        <v>44593.29993055556</v>
       </c>
       <c r="S10" s="11" t="n">
-        <v>44593.7722337963</v>
-      </c>
-      <c r="T10" s="10" t="n">
+        <v>44593.29997685185</v>
+      </c>
+      <c r="T10" s="11" t="n">
+        <v>44593.56390046296</v>
+      </c>
+      <c r="U10" s="10" t="n">
         <v>0.01409722222222222</v>
       </c>
-      <c r="U10" s="10" t="n">
+      <c r="V10" s="10" t="n">
         <v>0.02231481481481482</v>
       </c>
-      <c r="V10" s="10" t="n">
-        <v>4.629629629629629e-05</v>
-      </c>
       <c r="W10" s="10" t="n">
-        <v>0.2639236111111111</v>
+        <v>0.004409722222222222</v>
       </c>
       <c r="X10" s="10" t="n">
+        <v>0.03538194444444445</v>
+      </c>
+      <c r="Y10" s="10" t="n">
         <v>0.008472222222222223</v>
       </c>
-      <c r="Y10" s="10" t="n">
+      <c r="Z10" s="10" t="n">
         <v>0.09859953703703704</v>
       </c>
-      <c r="Z10" s="10" t="n">
+      <c r="AA10" s="10" t="n">
         <v>0.4472453703703704</v>
       </c>
     </row>
@@ -1244,61 +1541,66 @@
       </c>
       <c r="H11" s="5" t="inlineStr">
         <is>
+          <t>13075-7253</t>
+        </is>
+      </c>
+      <c r="I11" s="5" t="inlineStr">
+        <is>
           <t>SMK294</t>
         </is>
       </c>
-      <c r="I11" s="11" t="n">
-        <v>44593.19931712963</v>
-      </c>
       <c r="J11" s="11" t="n">
-        <v>44593.20748842593</v>
+        <v>44592.9909837963</v>
       </c>
       <c r="K11" s="11" t="n">
-        <v>44593.2153125</v>
+        <v>44592.99915509259</v>
       </c>
       <c r="L11" s="11" t="n">
-        <v>44593.23856481481</v>
+        <v>44593.00697916667</v>
       </c>
       <c r="M11" s="11" t="n">
-        <v>44593.24163194445</v>
+        <v>44593.03023148148</v>
       </c>
       <c r="N11" s="11" t="n">
-        <v>44593.26526620371</v>
+        <v>44593.03329861111</v>
       </c>
       <c r="O11" s="11" t="n">
-        <v>44593.27236111111</v>
+        <v>44593.05693287037</v>
       </c>
       <c r="P11" s="11" t="n">
-        <v>44593.28354166666</v>
+        <v>44593.06402777778</v>
       </c>
       <c r="Q11" s="11" t="n">
-        <v>44593.2899537037</v>
+        <v>44593.07520833334</v>
       </c>
       <c r="R11" s="11" t="n">
-        <v>44593.29311342593</v>
+        <v>44593.08162037037</v>
       </c>
       <c r="S11" s="11" t="n">
-        <v>44593.32475694444</v>
-      </c>
-      <c r="T11" s="10" t="n">
+        <v>44593.08478009259</v>
+      </c>
+      <c r="T11" s="11" t="n">
+        <v>44593.11642361111</v>
+      </c>
+      <c r="U11" s="10" t="n">
         <v>0.01599537037037037</v>
       </c>
-      <c r="U11" s="10" t="n">
+      <c r="V11" s="10" t="n">
         <v>0.02325231481481482</v>
       </c>
-      <c r="V11" s="10" t="n">
-        <v>0.003159722222222222</v>
-      </c>
       <c r="W11" s="10" t="n">
-        <v>0.03164351851851852</v>
+        <v>0.00306712962962963</v>
       </c>
       <c r="X11" s="10" t="n">
+        <v>0.02363425925925926</v>
+      </c>
+      <c r="Y11" s="10" t="n">
         <v>0.01827546296296296</v>
       </c>
-      <c r="Y11" s="10" t="n">
+      <c r="Z11" s="10" t="n">
         <v>0.006412037037037037</v>
       </c>
-      <c r="Z11" s="10" t="n">
+      <c r="AA11" s="10" t="n">
         <v>0.1254398148148148</v>
       </c>
     </row>
@@ -1334,10 +1636,14 @@
       </c>
       <c r="H12" s="5" t="inlineStr">
         <is>
+          <t>13075-7239</t>
+        </is>
+      </c>
+      <c r="I12" s="5" t="inlineStr">
+        <is>
           <t>SNC949</t>
         </is>
       </c>
-      <c r="I12" s="5" t="inlineStr"/>
       <c r="J12" s="5" t="inlineStr"/>
       <c r="K12" s="5" t="inlineStr"/>
       <c r="L12" s="5" t="inlineStr"/>
@@ -1348,13 +1654,14 @@
       <c r="Q12" s="5" t="inlineStr"/>
       <c r="R12" s="5" t="inlineStr"/>
       <c r="S12" s="5" t="inlineStr"/>
-      <c r="T12" s="10" t="inlineStr"/>
+      <c r="T12" s="5" t="inlineStr"/>
       <c r="U12" s="10" t="inlineStr"/>
       <c r="V12" s="10" t="inlineStr"/>
       <c r="W12" s="10" t="inlineStr"/>
       <c r="X12" s="10" t="inlineStr"/>
       <c r="Y12" s="10" t="inlineStr"/>
       <c r="Z12" s="10" t="inlineStr"/>
+      <c r="AA12" s="10" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="8" t="n">
@@ -1388,10 +1695,14 @@
       </c>
       <c r="H13" s="5" t="inlineStr">
         <is>
+          <t>13075-7240</t>
+        </is>
+      </c>
+      <c r="I13" s="5" t="inlineStr">
+        <is>
           <t>SNC949</t>
         </is>
       </c>
-      <c r="I13" s="5" t="inlineStr"/>
       <c r="J13" s="5" t="inlineStr"/>
       <c r="K13" s="5" t="inlineStr"/>
       <c r="L13" s="5" t="inlineStr"/>
@@ -1402,13 +1713,14 @@
       <c r="Q13" s="5" t="inlineStr"/>
       <c r="R13" s="5" t="inlineStr"/>
       <c r="S13" s="5" t="inlineStr"/>
-      <c r="T13" s="10" t="inlineStr"/>
+      <c r="T13" s="5" t="inlineStr"/>
       <c r="U13" s="10" t="inlineStr"/>
       <c r="V13" s="10" t="inlineStr"/>
       <c r="W13" s="10" t="inlineStr"/>
       <c r="X13" s="10" t="inlineStr"/>
       <c r="Y13" s="10" t="inlineStr"/>
       <c r="Z13" s="10" t="inlineStr"/>
+      <c r="AA13" s="10" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="8" t="n">
@@ -1442,61 +1754,66 @@
       </c>
       <c r="H14" s="5" t="inlineStr">
         <is>
+          <t>13075-7238</t>
+        </is>
+      </c>
+      <c r="I14" s="5" t="inlineStr">
+        <is>
           <t>SMK294</t>
         </is>
       </c>
-      <c r="I14" s="11" t="n">
-        <v>44592.5490625</v>
-      </c>
       <c r="J14" s="11" t="n">
-        <v>44592.54908564815</v>
+        <v>44592.34072916667</v>
       </c>
       <c r="K14" s="11" t="n">
-        <v>44592.55300925926</v>
+        <v>44592.34075231481</v>
       </c>
       <c r="L14" s="11" t="n">
-        <v>44592.57943287037</v>
+        <v>44592.34467592592</v>
       </c>
       <c r="M14" s="11" t="n">
-        <v>44592.58581018518</v>
+        <v>44592.37109953703</v>
       </c>
       <c r="N14" s="11" t="n">
-        <v>44592.61785879629</v>
+        <v>44592.37747685185</v>
       </c>
       <c r="O14" s="11" t="n">
-        <v>44592.61790509259</v>
+        <v>44592.40952546296</v>
       </c>
       <c r="P14" s="11" t="n">
-        <v>44592.64680555555</v>
+        <v>44592.40957175926</v>
       </c>
       <c r="Q14" s="11" t="n">
-        <v>44592.66866898148</v>
+        <v>44592.43847222222</v>
       </c>
       <c r="R14" s="11" t="n">
-        <v>44592.6687037037</v>
+        <v>44592.46033564815</v>
       </c>
       <c r="S14" s="11" t="n">
-        <v>44592.66873842593</v>
-      </c>
-      <c r="T14" s="10" t="n">
+        <v>44592.46037037037</v>
+      </c>
+      <c r="T14" s="11" t="n">
+        <v>44592.46040509259</v>
+      </c>
+      <c r="U14" s="10" t="n">
         <v>0.003946759259259259</v>
       </c>
-      <c r="U14" s="10" t="n">
+      <c r="V14" s="10" t="n">
         <v>0.02642361111111111</v>
       </c>
-      <c r="V14" s="10" t="n">
-        <v>3.472222222222222e-05</v>
-      </c>
       <c r="W14" s="10" t="n">
-        <v>3.472222222222222e-05</v>
+        <v>0.006377314814814815</v>
       </c>
       <c r="X14" s="10" t="n">
+        <v>0.03204861111111111</v>
+      </c>
+      <c r="Y14" s="10" t="n">
         <v>0.02894675925925926</v>
       </c>
-      <c r="Y14" s="10" t="n">
+      <c r="Z14" s="10" t="n">
         <v>0.02186342592592593</v>
       </c>
-      <c r="Z14" s="10" t="n">
+      <c r="AA14" s="10" t="n">
         <v>0.1196759259259259</v>
       </c>
     </row>
@@ -1512,7 +1829,7 @@
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>GENERADA</t>
+          <t>NOTIFICADA</t>
         </is>
       </c>
       <c r="E15" s="5" t="inlineStr">
@@ -1532,10 +1849,14 @@
       </c>
       <c r="H15" s="5" t="inlineStr">
         <is>
+          <t>13075-7235</t>
+        </is>
+      </c>
+      <c r="I15" s="5" t="inlineStr">
+        <is>
           <t>SJQ652</t>
         </is>
       </c>
-      <c r="I15" s="5" t="inlineStr"/>
       <c r="J15" s="5" t="inlineStr"/>
       <c r="K15" s="5" t="inlineStr"/>
       <c r="L15" s="5" t="inlineStr"/>
@@ -1546,13 +1867,14 @@
       <c r="Q15" s="5" t="inlineStr"/>
       <c r="R15" s="5" t="inlineStr"/>
       <c r="S15" s="5" t="inlineStr"/>
-      <c r="T15" s="10" t="inlineStr"/>
+      <c r="T15" s="5" t="inlineStr"/>
       <c r="U15" s="10" t="inlineStr"/>
       <c r="V15" s="10" t="inlineStr"/>
       <c r="W15" s="10" t="inlineStr"/>
       <c r="X15" s="10" t="inlineStr"/>
       <c r="Y15" s="10" t="inlineStr"/>
       <c r="Z15" s="10" t="inlineStr"/>
+      <c r="AA15" s="10" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="8" t="n">
@@ -1586,10 +1908,14 @@
       </c>
       <c r="H16" s="5" t="inlineStr">
         <is>
+          <t>13075-7241</t>
+        </is>
+      </c>
+      <c r="I16" s="5" t="inlineStr">
+        <is>
           <t>SUC236</t>
         </is>
       </c>
-      <c r="I16" s="5" t="inlineStr"/>
       <c r="J16" s="5" t="inlineStr"/>
       <c r="K16" s="5" t="inlineStr"/>
       <c r="L16" s="5" t="inlineStr"/>
@@ -1600,13 +1926,14 @@
       <c r="Q16" s="5" t="inlineStr"/>
       <c r="R16" s="5" t="inlineStr"/>
       <c r="S16" s="5" t="inlineStr"/>
-      <c r="T16" s="10" t="inlineStr"/>
+      <c r="T16" s="5" t="inlineStr"/>
       <c r="U16" s="10" t="inlineStr"/>
       <c r="V16" s="10" t="inlineStr"/>
       <c r="W16" s="10" t="inlineStr"/>
       <c r="X16" s="10" t="inlineStr"/>
       <c r="Y16" s="10" t="inlineStr"/>
       <c r="Z16" s="10" t="inlineStr"/>
+      <c r="AA16" s="10" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="8" t="n">
@@ -1640,10 +1967,14 @@
       </c>
       <c r="H17" s="5" t="inlineStr">
         <is>
+          <t>13075-7242</t>
+        </is>
+      </c>
+      <c r="I17" s="5" t="inlineStr">
+        <is>
           <t>THY168</t>
         </is>
       </c>
-      <c r="I17" s="5" t="inlineStr"/>
       <c r="J17" s="5" t="inlineStr"/>
       <c r="K17" s="5" t="inlineStr"/>
       <c r="L17" s="5" t="inlineStr"/>
@@ -1654,13 +1985,14 @@
       <c r="Q17" s="5" t="inlineStr"/>
       <c r="R17" s="5" t="inlineStr"/>
       <c r="S17" s="5" t="inlineStr"/>
-      <c r="T17" s="10" t="inlineStr"/>
+      <c r="T17" s="5" t="inlineStr"/>
       <c r="U17" s="10" t="inlineStr"/>
       <c r="V17" s="10" t="inlineStr"/>
       <c r="W17" s="10" t="inlineStr"/>
       <c r="X17" s="10" t="inlineStr"/>
       <c r="Y17" s="10" t="inlineStr"/>
       <c r="Z17" s="10" t="inlineStr"/>
+      <c r="AA17" s="10" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="8" t="n">
@@ -1674,7 +2006,7 @@
       </c>
       <c r="D18" s="5" t="inlineStr">
         <is>
-          <t>ACEPTADA</t>
+          <t>FINALIZADA</t>
         </is>
       </c>
       <c r="E18" s="5" t="inlineStr">
@@ -1694,41 +2026,68 @@
       </c>
       <c r="H18" s="5" t="inlineStr">
         <is>
+          <t>13043-1896</t>
+        </is>
+      </c>
+      <c r="I18" s="5" t="inlineStr">
+        <is>
           <t>SMK294</t>
         </is>
       </c>
-      <c r="I18" s="11" t="n">
-        <v>44592.66925925926</v>
-      </c>
       <c r="J18" s="11" t="n">
-        <v>44592.66930555556</v>
+        <v>44592.46092592592</v>
       </c>
       <c r="K18" s="11" t="n">
-        <v>44592.66967592593</v>
+        <v>44592.46097222222</v>
       </c>
       <c r="L18" s="11" t="n">
-        <v>44592.70476851852</v>
+        <v>44592.46134259259</v>
       </c>
       <c r="M18" s="11" t="n">
-        <v>44592.70512731482</v>
-      </c>
-      <c r="N18" s="5" t="inlineStr"/>
-      <c r="O18" s="5" t="inlineStr"/>
-      <c r="P18" s="5" t="inlineStr"/>
-      <c r="Q18" s="5" t="inlineStr"/>
-      <c r="R18" s="5" t="inlineStr"/>
-      <c r="S18" s="5" t="inlineStr"/>
-      <c r="T18" s="10" t="n">
+        <v>44592.49643518519</v>
+      </c>
+      <c r="N18" s="11" t="n">
+        <v>44592.49679398148</v>
+      </c>
+      <c r="O18" s="11" t="n">
+        <v>44592.53155092592</v>
+      </c>
+      <c r="P18" s="11" t="n">
+        <v>44592.54871527778</v>
+      </c>
+      <c r="Q18" s="11" t="n">
+        <v>44592.55466435185</v>
+      </c>
+      <c r="R18" s="11" t="n">
+        <v>44592.59570601852</v>
+      </c>
+      <c r="S18" s="11" t="n">
+        <v>44592.63362268519</v>
+      </c>
+      <c r="T18" s="11" t="n">
+        <v>44592.63365740741</v>
+      </c>
+      <c r="U18" s="10" t="n">
         <v>0.0004166666666666667</v>
       </c>
-      <c r="U18" s="10" t="n">
+      <c r="V18" s="10" t="n">
         <v>0.03509259259259259</v>
       </c>
-      <c r="V18" s="10" t="inlineStr"/>
-      <c r="W18" s="10" t="inlineStr"/>
-      <c r="X18" s="10" t="inlineStr"/>
-      <c r="Y18" s="10" t="inlineStr"/>
-      <c r="Z18" s="10" t="inlineStr"/>
+      <c r="W18" s="10" t="n">
+        <v>0.0003587962962962963</v>
+      </c>
+      <c r="X18" s="10" t="n">
+        <v>0.03475694444444444</v>
+      </c>
+      <c r="Y18" s="10" t="n">
+        <v>0.02311342592592593</v>
+      </c>
+      <c r="Z18" s="10" t="n">
+        <v>0.04104166666666666</v>
+      </c>
+      <c r="AA18" s="10" t="n">
+        <v>0.1727314814814815</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="n">
@@ -1742,7 +2101,7 @@
       </c>
       <c r="D19" s="5" t="inlineStr">
         <is>
-          <t>NOTIFICADA</t>
+          <t>FINALIZADA</t>
         </is>
       </c>
       <c r="E19" s="5" t="inlineStr">
@@ -1762,27 +2121,68 @@
       </c>
       <c r="H19" s="5" t="inlineStr">
         <is>
+          <t>13075-7243</t>
+        </is>
+      </c>
+      <c r="I19" s="5" t="inlineStr">
+        <is>
           <t>SMK294</t>
         </is>
       </c>
-      <c r="I19" s="5" t="inlineStr"/>
-      <c r="J19" s="5" t="inlineStr"/>
-      <c r="K19" s="5" t="inlineStr"/>
-      <c r="L19" s="5" t="inlineStr"/>
-      <c r="M19" s="5" t="inlineStr"/>
-      <c r="N19" s="5" t="inlineStr"/>
-      <c r="O19" s="5" t="inlineStr"/>
-      <c r="P19" s="5" t="inlineStr"/>
-      <c r="Q19" s="5" t="inlineStr"/>
-      <c r="R19" s="5" t="inlineStr"/>
-      <c r="S19" s="5" t="inlineStr"/>
-      <c r="T19" s="10" t="inlineStr"/>
-      <c r="U19" s="10" t="inlineStr"/>
-      <c r="V19" s="10" t="inlineStr"/>
-      <c r="W19" s="10" t="inlineStr"/>
-      <c r="X19" s="10" t="inlineStr"/>
-      <c r="Y19" s="10" t="inlineStr"/>
-      <c r="Z19" s="10" t="inlineStr"/>
+      <c r="J19" s="11" t="n">
+        <v>44592.63383101852</v>
+      </c>
+      <c r="K19" s="11" t="n">
+        <v>44592.63386574074</v>
+      </c>
+      <c r="L19" s="11" t="n">
+        <v>44592.63408564815</v>
+      </c>
+      <c r="M19" s="11" t="n">
+        <v>44592.67883101852</v>
+      </c>
+      <c r="N19" s="11" t="n">
+        <v>44592.69200231481</v>
+      </c>
+      <c r="O19" s="11" t="n">
+        <v>44592.72039351852</v>
+      </c>
+      <c r="P19" s="11" t="n">
+        <v>44592.72408564815</v>
+      </c>
+      <c r="Q19" s="11" t="n">
+        <v>44592.74607638889</v>
+      </c>
+      <c r="R19" s="11" t="n">
+        <v>44593.41204861111</v>
+      </c>
+      <c r="S19" s="11" t="n">
+        <v>44593.41231481481</v>
+      </c>
+      <c r="T19" s="11" t="n">
+        <v>44593.4131712963</v>
+      </c>
+      <c r="U19" s="10" t="n">
+        <v>0.0002546296296296296</v>
+      </c>
+      <c r="V19" s="10" t="n">
+        <v>0.04474537037037037</v>
+      </c>
+      <c r="W19" s="10" t="n">
+        <v>0.0131712962962963</v>
+      </c>
+      <c r="X19" s="10" t="n">
+        <v>0.0283912037037037</v>
+      </c>
+      <c r="Y19" s="10" t="n">
+        <v>0.02568287037037037</v>
+      </c>
+      <c r="Z19" s="10" t="n">
+        <v>0.6659722222222222</v>
+      </c>
+      <c r="AA19" s="10" t="n">
+        <v>0.7793402777777778</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="n">
@@ -1796,7 +2196,7 @@
       </c>
       <c r="D20" s="5" t="inlineStr">
         <is>
-          <t>GENERADA</t>
+          <t>NOTIFICADA</t>
         </is>
       </c>
       <c r="E20" s="5" t="inlineStr">
@@ -1816,10 +2216,14 @@
       </c>
       <c r="H20" s="5" t="inlineStr">
         <is>
+          <t>13043-1897</t>
+        </is>
+      </c>
+      <c r="I20" s="5" t="inlineStr">
+        <is>
           <t>SJQ652</t>
         </is>
       </c>
-      <c r="I20" s="5" t="inlineStr"/>
       <c r="J20" s="5" t="inlineStr"/>
       <c r="K20" s="5" t="inlineStr"/>
       <c r="L20" s="5" t="inlineStr"/>
@@ -1830,13 +2234,14 @@
       <c r="Q20" s="5" t="inlineStr"/>
       <c r="R20" s="5" t="inlineStr"/>
       <c r="S20" s="5" t="inlineStr"/>
-      <c r="T20" s="10" t="inlineStr"/>
+      <c r="T20" s="5" t="inlineStr"/>
       <c r="U20" s="10" t="inlineStr"/>
       <c r="V20" s="10" t="inlineStr"/>
       <c r="W20" s="10" t="inlineStr"/>
       <c r="X20" s="10" t="inlineStr"/>
       <c r="Y20" s="10" t="inlineStr"/>
       <c r="Z20" s="10" t="inlineStr"/>
+      <c r="AA20" s="10" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="8" t="n">
@@ -1870,61 +2275,66 @@
       </c>
       <c r="H21" s="5" t="inlineStr">
         <is>
+          <t>13075-7252</t>
+        </is>
+      </c>
+      <c r="I21" s="5" t="inlineStr">
+        <is>
           <t>SKF030</t>
         </is>
       </c>
-      <c r="I21" s="11" t="n">
-        <v>44593.06472222223</v>
-      </c>
       <c r="J21" s="11" t="n">
-        <v>44593.07277777778</v>
+        <v>44592.85638888889</v>
       </c>
       <c r="K21" s="11" t="n">
-        <v>44593.08125</v>
+        <v>44592.86444444444</v>
       </c>
       <c r="L21" s="11" t="n">
-        <v>44593.10590277778</v>
+        <v>44592.87291666667</v>
       </c>
       <c r="M21" s="11" t="n">
-        <v>44593.12325231481</v>
+        <v>44592.89756944445</v>
       </c>
       <c r="N21" s="11" t="n">
-        <v>44593.14835648148</v>
+        <v>44592.91491898148</v>
       </c>
       <c r="O21" s="11" t="n">
-        <v>44593.16928240741</v>
+        <v>44592.94002314815</v>
       </c>
       <c r="P21" s="11" t="n">
-        <v>44593.16931712963</v>
+        <v>44592.96094907408</v>
       </c>
       <c r="Q21" s="11" t="n">
-        <v>44593.19916666667</v>
+        <v>44592.9609837963</v>
       </c>
       <c r="R21" s="11" t="n">
-        <v>44593.19920138889</v>
+        <v>44592.99083333334</v>
       </c>
       <c r="S21" s="11" t="n">
-        <v>44593.19924768519</v>
-      </c>
-      <c r="T21" s="10" t="n">
+        <v>44592.99086805555</v>
+      </c>
+      <c r="T21" s="11" t="n">
+        <v>44592.99091435185</v>
+      </c>
+      <c r="U21" s="10" t="n">
         <v>0.01652777777777778</v>
       </c>
-      <c r="U21" s="10" t="n">
+      <c r="V21" s="10" t="n">
         <v>0.02465277777777778</v>
       </c>
-      <c r="V21" s="10" t="n">
-        <v>3.472222222222222e-05</v>
-      </c>
       <c r="W21" s="10" t="n">
-        <v>4.629629629629629e-05</v>
+        <v>0.01734953703703704</v>
       </c>
       <c r="X21" s="10" t="n">
+        <v>0.02510416666666667</v>
+      </c>
+      <c r="Y21" s="10" t="n">
         <v>0.02096064814814815</v>
       </c>
-      <c r="Y21" s="10" t="n">
+      <c r="Z21" s="10" t="n">
         <v>0.02984953703703704</v>
       </c>
-      <c r="Z21" s="10" t="n">
+      <c r="AA21" s="10" t="n">
         <v>0.134525462962963</v>
       </c>
     </row>
@@ -1960,10 +2370,14 @@
       </c>
       <c r="H22" s="5" t="inlineStr">
         <is>
+          <t>13075-7249</t>
+        </is>
+      </c>
+      <c r="I22" s="5" t="inlineStr">
+        <is>
           <t>SNC949</t>
         </is>
       </c>
-      <c r="I22" s="5" t="inlineStr"/>
       <c r="J22" s="5" t="inlineStr"/>
       <c r="K22" s="5" t="inlineStr"/>
       <c r="L22" s="5" t="inlineStr"/>
@@ -1974,13 +2388,14 @@
       <c r="Q22" s="5" t="inlineStr"/>
       <c r="R22" s="5" t="inlineStr"/>
       <c r="S22" s="5" t="inlineStr"/>
-      <c r="T22" s="10" t="inlineStr"/>
+      <c r="T22" s="5" t="inlineStr"/>
       <c r="U22" s="10" t="inlineStr"/>
       <c r="V22" s="10" t="inlineStr"/>
       <c r="W22" s="10" t="inlineStr"/>
       <c r="X22" s="10" t="inlineStr"/>
       <c r="Y22" s="10" t="inlineStr"/>
       <c r="Z22" s="10" t="inlineStr"/>
+      <c r="AA22" s="10" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="8" t="n">
@@ -2014,10 +2429,14 @@
       </c>
       <c r="H23" s="5" t="inlineStr">
         <is>
+          <t>13075-7250</t>
+        </is>
+      </c>
+      <c r="I23" s="5" t="inlineStr">
+        <is>
           <t>SNC949</t>
         </is>
       </c>
-      <c r="I23" s="5" t="inlineStr"/>
       <c r="J23" s="5" t="inlineStr"/>
       <c r="K23" s="5" t="inlineStr"/>
       <c r="L23" s="5" t="inlineStr"/>
@@ -2028,13 +2447,14 @@
       <c r="Q23" s="5" t="inlineStr"/>
       <c r="R23" s="5" t="inlineStr"/>
       <c r="S23" s="5" t="inlineStr"/>
-      <c r="T23" s="10" t="inlineStr"/>
+      <c r="T23" s="5" t="inlineStr"/>
       <c r="U23" s="10" t="inlineStr"/>
       <c r="V23" s="10" t="inlineStr"/>
       <c r="W23" s="10" t="inlineStr"/>
       <c r="X23" s="10" t="inlineStr"/>
       <c r="Y23" s="10" t="inlineStr"/>
       <c r="Z23" s="10" t="inlineStr"/>
+      <c r="AA23" s="10" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="8" t="n">
@@ -2048,7 +2468,7 @@
       </c>
       <c r="D24" s="5" t="inlineStr">
         <is>
-          <t>GENERADA</t>
+          <t>FINALIZADA</t>
         </is>
       </c>
       <c r="E24" s="5" t="inlineStr">
@@ -2068,27 +2488,68 @@
       </c>
       <c r="H24" s="5" t="inlineStr">
         <is>
+          <t>13075-7257</t>
+        </is>
+      </c>
+      <c r="I24" s="5" t="inlineStr">
+        <is>
           <t>SMK294</t>
         </is>
       </c>
-      <c r="I24" s="5" t="inlineStr"/>
-      <c r="J24" s="5" t="inlineStr"/>
-      <c r="K24" s="5" t="inlineStr"/>
-      <c r="L24" s="5" t="inlineStr"/>
-      <c r="M24" s="5" t="inlineStr"/>
-      <c r="N24" s="5" t="inlineStr"/>
-      <c r="O24" s="5" t="inlineStr"/>
-      <c r="P24" s="5" t="inlineStr"/>
-      <c r="Q24" s="5" t="inlineStr"/>
-      <c r="R24" s="5" t="inlineStr"/>
-      <c r="S24" s="5" t="inlineStr"/>
-      <c r="T24" s="10" t="inlineStr"/>
-      <c r="U24" s="10" t="inlineStr"/>
-      <c r="V24" s="10" t="inlineStr"/>
-      <c r="W24" s="10" t="inlineStr"/>
-      <c r="X24" s="10" t="inlineStr"/>
-      <c r="Y24" s="10" t="inlineStr"/>
-      <c r="Z24" s="10" t="inlineStr"/>
+      <c r="J24" s="11" t="n">
+        <v>44593.42186342592</v>
+      </c>
+      <c r="K24" s="11" t="n">
+        <v>44593.42208333333</v>
+      </c>
+      <c r="L24" s="11" t="n">
+        <v>44593.42231481482</v>
+      </c>
+      <c r="M24" s="11" t="n">
+        <v>44593.44414351852</v>
+      </c>
+      <c r="N24" s="11" t="n">
+        <v>44593.45122685185</v>
+      </c>
+      <c r="O24" s="11" t="n">
+        <v>44593.48322916667</v>
+      </c>
+      <c r="P24" s="11" t="n">
+        <v>44593.48331018518</v>
+      </c>
+      <c r="Q24" s="11" t="n">
+        <v>44593.52699074074</v>
+      </c>
+      <c r="R24" s="11" t="n">
+        <v>44593.56614583333</v>
+      </c>
+      <c r="S24" s="11" t="n">
+        <v>44593.56619212963</v>
+      </c>
+      <c r="T24" s="11" t="n">
+        <v>44593.56622685185</v>
+      </c>
+      <c r="U24" s="10" t="n">
+        <v>0.0004513888888888889</v>
+      </c>
+      <c r="V24" s="10" t="n">
+        <v>0.0218287037037037</v>
+      </c>
+      <c r="W24" s="10" t="n">
+        <v>0.007083333333333333</v>
+      </c>
+      <c r="X24" s="10" t="n">
+        <v>0.03200231481481482</v>
+      </c>
+      <c r="Y24" s="10" t="n">
+        <v>0.04376157407407407</v>
+      </c>
+      <c r="Z24" s="10" t="n">
+        <v>0.0391550925925926</v>
+      </c>
+      <c r="AA24" s="10" t="n">
+        <v>0.1443634259259259</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="n">
@@ -2122,10 +2583,14 @@
       </c>
       <c r="H25" s="5" t="inlineStr">
         <is>
+          <t>13043-1900</t>
+        </is>
+      </c>
+      <c r="I25" s="5" t="inlineStr">
+        <is>
           <t>SUC236</t>
         </is>
       </c>
-      <c r="I25" s="5" t="inlineStr"/>
       <c r="J25" s="5" t="inlineStr"/>
       <c r="K25" s="5" t="inlineStr"/>
       <c r="L25" s="5" t="inlineStr"/>
@@ -2136,13 +2601,14 @@
       <c r="Q25" s="5" t="inlineStr"/>
       <c r="R25" s="5" t="inlineStr"/>
       <c r="S25" s="5" t="inlineStr"/>
-      <c r="T25" s="10" t="inlineStr"/>
+      <c r="T25" s="5" t="inlineStr"/>
       <c r="U25" s="10" t="inlineStr"/>
       <c r="V25" s="10" t="inlineStr"/>
       <c r="W25" s="10" t="inlineStr"/>
       <c r="X25" s="10" t="inlineStr"/>
       <c r="Y25" s="10" t="inlineStr"/>
       <c r="Z25" s="10" t="inlineStr"/>
+      <c r="AA25" s="10" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="8" t="n">
@@ -2176,10 +2642,14 @@
       </c>
       <c r="H26" s="5" t="inlineStr">
         <is>
+          <t>13075-7266</t>
+        </is>
+      </c>
+      <c r="I26" s="5" t="inlineStr">
+        <is>
           <t>SNC949</t>
         </is>
       </c>
-      <c r="I26" s="5" t="inlineStr"/>
       <c r="J26" s="5" t="inlineStr"/>
       <c r="K26" s="5" t="inlineStr"/>
       <c r="L26" s="5" t="inlineStr"/>
@@ -2190,13 +2660,14 @@
       <c r="Q26" s="5" t="inlineStr"/>
       <c r="R26" s="5" t="inlineStr"/>
       <c r="S26" s="5" t="inlineStr"/>
-      <c r="T26" s="10" t="inlineStr"/>
+      <c r="T26" s="5" t="inlineStr"/>
       <c r="U26" s="10" t="inlineStr"/>
       <c r="V26" s="10" t="inlineStr"/>
       <c r="W26" s="10" t="inlineStr"/>
       <c r="X26" s="10" t="inlineStr"/>
       <c r="Y26" s="10" t="inlineStr"/>
       <c r="Z26" s="10" t="inlineStr"/>
+      <c r="AA26" s="10" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="8" t="n">
@@ -2230,10 +2701,14 @@
       </c>
       <c r="H27" s="5" t="inlineStr">
         <is>
+          <t>13075-7267</t>
+        </is>
+      </c>
+      <c r="I27" s="5" t="inlineStr">
+        <is>
           <t>SNC949</t>
         </is>
       </c>
-      <c r="I27" s="5" t="inlineStr"/>
       <c r="J27" s="5" t="inlineStr"/>
       <c r="K27" s="5" t="inlineStr"/>
       <c r="L27" s="5" t="inlineStr"/>
@@ -2244,13 +2719,14 @@
       <c r="Q27" s="5" t="inlineStr"/>
       <c r="R27" s="5" t="inlineStr"/>
       <c r="S27" s="5" t="inlineStr"/>
-      <c r="T27" s="10" t="inlineStr"/>
+      <c r="T27" s="5" t="inlineStr"/>
       <c r="U27" s="10" t="inlineStr"/>
       <c r="V27" s="10" t="inlineStr"/>
       <c r="W27" s="10" t="inlineStr"/>
       <c r="X27" s="10" t="inlineStr"/>
       <c r="Y27" s="10" t="inlineStr"/>
       <c r="Z27" s="10" t="inlineStr"/>
+      <c r="AA27" s="10" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="8" t="n">
@@ -2284,10 +2760,14 @@
       </c>
       <c r="H28" s="5" t="inlineStr">
         <is>
+          <t>13075-7268</t>
+        </is>
+      </c>
+      <c r="I28" s="5" t="inlineStr">
+        <is>
           <t>SNC949</t>
         </is>
       </c>
-      <c r="I28" s="5" t="inlineStr"/>
       <c r="J28" s="5" t="inlineStr"/>
       <c r="K28" s="5" t="inlineStr"/>
       <c r="L28" s="5" t="inlineStr"/>
@@ -2298,13 +2778,14 @@
       <c r="Q28" s="5" t="inlineStr"/>
       <c r="R28" s="5" t="inlineStr"/>
       <c r="S28" s="5" t="inlineStr"/>
-      <c r="T28" s="10" t="inlineStr"/>
+      <c r="T28" s="5" t="inlineStr"/>
       <c r="U28" s="10" t="inlineStr"/>
       <c r="V28" s="10" t="inlineStr"/>
       <c r="W28" s="10" t="inlineStr"/>
       <c r="X28" s="10" t="inlineStr"/>
       <c r="Y28" s="10" t="inlineStr"/>
       <c r="Z28" s="10" t="inlineStr"/>
+      <c r="AA28" s="10" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="8" t="n">
@@ -2338,61 +2819,66 @@
       </c>
       <c r="H29" s="5" t="inlineStr">
         <is>
+          <t>13075-7275</t>
+        </is>
+      </c>
+      <c r="I29" s="5" t="inlineStr">
+        <is>
           <t>SMK294</t>
         </is>
       </c>
-      <c r="I29" s="11" t="n">
-        <v>44594.0275925926</v>
-      </c>
       <c r="J29" s="11" t="n">
-        <v>44594.03430555556</v>
+        <v>44593.81925925926</v>
       </c>
       <c r="K29" s="11" t="n">
-        <v>44594.03677083334</v>
+        <v>44593.82597222222</v>
       </c>
       <c r="L29" s="11" t="n">
-        <v>44594.05946759259</v>
+        <v>44593.8284375</v>
       </c>
       <c r="M29" s="11" t="n">
-        <v>44594.07447916667</v>
+        <v>44593.85113425926</v>
       </c>
       <c r="N29" s="11" t="n">
-        <v>44594.10011574074</v>
+        <v>44593.86614583333</v>
       </c>
       <c r="O29" s="11" t="n">
-        <v>44594.10741898148</v>
+        <v>44593.89178240741</v>
       </c>
       <c r="P29" s="11" t="n">
-        <v>44594.11616898148</v>
+        <v>44593.89908564815</v>
       </c>
       <c r="Q29" s="11" t="n">
-        <v>44594.17590277778</v>
+        <v>44593.90783564815</v>
       </c>
       <c r="R29" s="11" t="n">
-        <v>44594.18826388889</v>
+        <v>44593.96756944444</v>
       </c>
       <c r="S29" s="11" t="n">
-        <v>44594.22226851852</v>
-      </c>
-      <c r="T29" s="10" t="n">
+        <v>44593.97993055556</v>
+      </c>
+      <c r="T29" s="11" t="n">
+        <v>44594.01393518518</v>
+      </c>
+      <c r="U29" s="10" t="n">
         <v>0.00917824074074074</v>
       </c>
-      <c r="U29" s="10" t="n">
+      <c r="V29" s="10" t="n">
         <v>0.02269675925925926</v>
       </c>
-      <c r="V29" s="10" t="n">
-        <v>0.01236111111111111</v>
-      </c>
       <c r="W29" s="10" t="n">
-        <v>0.03400462962962963</v>
+        <v>0.01501157407407407</v>
       </c>
       <c r="X29" s="10" t="n">
+        <v>0.02563657407407408</v>
+      </c>
+      <c r="Y29" s="10" t="n">
         <v>0.01605324074074074</v>
       </c>
-      <c r="Y29" s="10" t="n">
+      <c r="Z29" s="10" t="n">
         <v>0.0597337962962963</v>
       </c>
-      <c r="Z29" s="10" t="n">
+      <c r="AA29" s="10" t="n">
         <v>0.1946759259259259</v>
       </c>
     </row>
@@ -2428,61 +2914,66 @@
       </c>
       <c r="H30" s="5" t="inlineStr">
         <is>
+          <t>13075-7276</t>
+        </is>
+      </c>
+      <c r="I30" s="5" t="inlineStr">
+        <is>
           <t>SMK294</t>
         </is>
       </c>
-      <c r="I30" s="11" t="n">
-        <v>44594.22258101852</v>
-      </c>
       <c r="J30" s="11" t="n">
-        <v>44594.2275</v>
+        <v>44594.01424768518</v>
       </c>
       <c r="K30" s="11" t="n">
-        <v>44594.25107638889</v>
+        <v>44594.01916666667</v>
       </c>
       <c r="L30" s="11" t="n">
-        <v>44594.27774305556</v>
+        <v>44594.04274305556</v>
       </c>
       <c r="M30" s="11" t="n">
-        <v>44594.2890162037</v>
+        <v>44594.06940972222</v>
       </c>
       <c r="N30" s="11" t="n">
-        <v>44594.32438657407</v>
+        <v>44594.08068287037</v>
       </c>
       <c r="O30" s="11" t="n">
-        <v>44594.32672453704</v>
+        <v>44594.11605324074</v>
       </c>
       <c r="P30" s="11" t="n">
-        <v>44594.33759259259</v>
+        <v>44594.1183912037</v>
       </c>
       <c r="Q30" s="11" t="n">
-        <v>44594.38510416666</v>
+        <v>44594.12925925926</v>
       </c>
       <c r="R30" s="11" t="n">
-        <v>44594.90179398148</v>
+        <v>44594.17677083334</v>
       </c>
       <c r="S30" s="11" t="n">
-        <v>44594.95599537037</v>
-      </c>
-      <c r="T30" s="10" t="n">
+        <v>44594.69346064814</v>
+      </c>
+      <c r="T30" s="11" t="n">
+        <v>44594.74766203704</v>
+      </c>
+      <c r="U30" s="10" t="n">
         <v>0.02849537037037037</v>
       </c>
-      <c r="U30" s="10" t="n">
+      <c r="V30" s="10" t="n">
         <v>0.02666666666666667</v>
       </c>
-      <c r="V30" s="10" t="n">
-        <v>0.5166898148148148</v>
-      </c>
       <c r="W30" s="10" t="n">
-        <v>0.05420138888888889</v>
+        <v>0.01127314814814815</v>
       </c>
       <c r="X30" s="10" t="n">
+        <v>0.03537037037037037</v>
+      </c>
+      <c r="Y30" s="10" t="n">
         <v>0.01320601851851852</v>
       </c>
-      <c r="Y30" s="10" t="n">
+      <c r="Z30" s="10" t="n">
         <v>0.04751157407407407</v>
       </c>
-      <c r="Z30" s="10" t="n">
+      <c r="AA30" s="10" t="n">
         <v>0.7334143518518519</v>
       </c>
     </row>
@@ -2498,7 +2989,7 @@
       </c>
       <c r="D31" s="5" t="inlineStr">
         <is>
-          <t>ACEPTADA</t>
+          <t>FINALIZADA</t>
         </is>
       </c>
       <c r="E31" s="5" t="inlineStr">
@@ -2518,57 +3009,68 @@
       </c>
       <c r="H31" s="5" t="inlineStr">
         <is>
+          <t>13075-7277</t>
+        </is>
+      </c>
+      <c r="I31" s="5" t="inlineStr">
+        <is>
           <t>SMK294</t>
         </is>
       </c>
-      <c r="I31" s="11" t="n">
-        <v>44595.00659722222</v>
-      </c>
       <c r="J31" s="11" t="n">
-        <v>44595.01248842593</v>
+        <v>44594.79826388889</v>
       </c>
       <c r="K31" s="11" t="n">
-        <v>44595.01638888889</v>
+        <v>44594.80415509259</v>
       </c>
       <c r="L31" s="11" t="n">
-        <v>44595.03850694445</v>
+        <v>44594.80805555556</v>
       </c>
       <c r="M31" s="11" t="n">
-        <v>44595.05010416666</v>
+        <v>44594.83017361111</v>
       </c>
       <c r="N31" s="11" t="n">
-        <v>44595.0771875</v>
+        <v>44594.84177083334</v>
       </c>
       <c r="O31" s="11" t="n">
-        <v>44595.08902777778</v>
+        <v>44594.86885416666</v>
       </c>
       <c r="P31" s="11" t="n">
-        <v>44595.09603009259</v>
+        <v>44594.88069444444</v>
       </c>
       <c r="Q31" s="11" t="n">
-        <v>44595.1137962963</v>
+        <v>44594.88769675926</v>
       </c>
       <c r="R31" s="11" t="n">
-        <v>44595.11983796296</v>
-      </c>
-      <c r="S31" s="5" t="inlineStr"/>
-      <c r="T31" s="10" t="n">
+        <v>44594.90546296296</v>
+      </c>
+      <c r="S31" s="11" t="n">
+        <v>44594.91150462963</v>
+      </c>
+      <c r="T31" s="11" t="n">
+        <v>44594.94038194444</v>
+      </c>
+      <c r="U31" s="10" t="n">
         <v>0.009791666666666667</v>
       </c>
-      <c r="U31" s="10" t="n">
+      <c r="V31" s="10" t="n">
         <v>0.02211805555555555</v>
       </c>
-      <c r="V31" s="10" t="n">
-        <v>0.006041666666666667</v>
-      </c>
-      <c r="W31" s="10" t="inlineStr"/>
+      <c r="W31" s="10" t="n">
+        <v>0.01159722222222222</v>
+      </c>
       <c r="X31" s="10" t="n">
+        <v>0.02708333333333333</v>
+      </c>
+      <c r="Y31" s="10" t="n">
         <v>0.01884259259259259</v>
       </c>
-      <c r="Y31" s="10" t="n">
+      <c r="Z31" s="10" t="n">
         <v>0.0177662037037037</v>
       </c>
-      <c r="Z31" s="10" t="inlineStr"/>
+      <c r="AA31" s="10" t="n">
+        <v>0.1421180555555556</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="n">
@@ -2602,61 +3104,66 @@
       </c>
       <c r="H32" s="5" t="inlineStr">
         <is>
+          <t>13043-1904</t>
+        </is>
+      </c>
+      <c r="I32" s="5" t="inlineStr">
+        <is>
           <t>SMK294</t>
         </is>
       </c>
-      <c r="I32" s="11" t="n">
-        <v>44594.17608796297</v>
-      </c>
       <c r="J32" s="11" t="n">
-        <v>44594.17612268519</v>
+        <v>44593.96775462963</v>
       </c>
       <c r="K32" s="11" t="n">
-        <v>44594.17631944444</v>
+        <v>44593.96778935185</v>
       </c>
       <c r="L32" s="11" t="n">
-        <v>44594.183125</v>
+        <v>44593.96798611111</v>
       </c>
       <c r="M32" s="11" t="n">
-        <v>44594.18815972222</v>
+        <v>44593.97479166667</v>
       </c>
       <c r="N32" s="11" t="n">
-        <v>44594.22234953703</v>
+        <v>44593.97982638889</v>
       </c>
       <c r="O32" s="11" t="n">
-        <v>44594.22760416667</v>
+        <v>44594.01401620371</v>
       </c>
       <c r="P32" s="11" t="n">
-        <v>44594.24314814815</v>
+        <v>44594.01927083333</v>
       </c>
       <c r="Q32" s="11" t="n">
-        <v>44594.25048611111</v>
+        <v>44594.03481481481</v>
       </c>
       <c r="R32" s="11" t="n">
-        <v>44594.2918287037</v>
+        <v>44594.04215277778</v>
       </c>
       <c r="S32" s="11" t="n">
-        <v>44594.291875</v>
-      </c>
-      <c r="T32" s="10" t="n">
+        <v>44594.08349537037</v>
+      </c>
+      <c r="T32" s="11" t="n">
+        <v>44594.08354166667</v>
+      </c>
+      <c r="U32" s="10" t="n">
         <v>0.0002314814814814815</v>
       </c>
-      <c r="U32" s="10" t="n">
+      <c r="V32" s="10" t="n">
         <v>0.006805555555555555</v>
       </c>
-      <c r="V32" s="10" t="n">
-        <v>0.04134259259259259</v>
-      </c>
       <c r="W32" s="10" t="n">
-        <v>4.629629629629629e-05</v>
+        <v>0.005034722222222223</v>
       </c>
       <c r="X32" s="10" t="n">
+        <v>0.03418981481481481</v>
+      </c>
+      <c r="Y32" s="10" t="n">
         <v>0.02079861111111111</v>
       </c>
-      <c r="Y32" s="10" t="n">
+      <c r="Z32" s="10" t="n">
         <v>0.007337962962962963</v>
       </c>
-      <c r="Z32" s="10" t="n">
+      <c r="AA32" s="10" t="n">
         <v>0.115787037037037</v>
       </c>
     </row>
@@ -2672,7 +3179,7 @@
       </c>
       <c r="D33" s="5" t="inlineStr">
         <is>
-          <t>GENERADA</t>
+          <t>NOTIFICADA</t>
         </is>
       </c>
       <c r="E33" s="5" t="inlineStr">
@@ -2692,10 +3199,14 @@
       </c>
       <c r="H33" s="5" t="inlineStr">
         <is>
+          <t>13075-7246</t>
+        </is>
+      </c>
+      <c r="I33" s="5" t="inlineStr">
+        <is>
           <t>SJQ652</t>
         </is>
       </c>
-      <c r="I33" s="5" t="inlineStr"/>
       <c r="J33" s="5" t="inlineStr"/>
       <c r="K33" s="5" t="inlineStr"/>
       <c r="L33" s="5" t="inlineStr"/>
@@ -2706,164 +3217,183 @@
       <c r="Q33" s="5" t="inlineStr"/>
       <c r="R33" s="5" t="inlineStr"/>
       <c r="S33" s="5" t="inlineStr"/>
-      <c r="T33" s="10" t="inlineStr"/>
+      <c r="T33" s="5" t="inlineStr"/>
       <c r="U33" s="10" t="inlineStr"/>
       <c r="V33" s="10" t="inlineStr"/>
       <c r="W33" s="10" t="inlineStr"/>
       <c r="X33" s="10" t="inlineStr"/>
       <c r="Y33" s="10" t="inlineStr"/>
       <c r="Z33" s="10" t="inlineStr"/>
+      <c r="AA33" s="10" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="8" t="n">
         <v>27</v>
       </c>
       <c r="B34" s="5" t="n">
-        <v>161361</v>
+        <v>161362</v>
       </c>
       <c r="C34" s="9" t="n">
         <v>44592</v>
       </c>
       <c r="D34" s="5" t="inlineStr">
         <is>
-          <t>GENERADA</t>
+          <t>FINALIZADA</t>
         </is>
       </c>
       <c r="E34" s="5" t="inlineStr">
         <is>
-          <t>ELKIN FABIAN GONZALEZ BUSTOS</t>
+          <t>FABIO ENRIQUE TORRES PANQUEBA</t>
         </is>
       </c>
       <c r="F34" s="5" t="inlineStr">
         <is>
-          <t>1071165330</t>
+          <t>1073503221</t>
         </is>
       </c>
       <c r="G34" s="5" t="inlineStr">
         <is>
-          <t>13075-7067</t>
+          <t>13043-1800</t>
         </is>
       </c>
       <c r="H34" s="5" t="inlineStr">
         <is>
-          <t>SJQ652</t>
-        </is>
-      </c>
-      <c r="I34" s="5" t="inlineStr"/>
-      <c r="J34" s="5" t="inlineStr"/>
-      <c r="K34" s="5" t="inlineStr"/>
-      <c r="L34" s="5" t="inlineStr"/>
-      <c r="M34" s="5" t="inlineStr"/>
-      <c r="N34" s="5" t="inlineStr"/>
-      <c r="O34" s="5" t="inlineStr"/>
-      <c r="P34" s="5" t="inlineStr"/>
-      <c r="Q34" s="5" t="inlineStr"/>
-      <c r="R34" s="5" t="inlineStr"/>
-      <c r="S34" s="5" t="inlineStr"/>
-      <c r="T34" s="10" t="inlineStr"/>
-      <c r="U34" s="10" t="inlineStr"/>
-      <c r="V34" s="10" t="inlineStr"/>
-      <c r="W34" s="10" t="inlineStr"/>
-      <c r="X34" s="10" t="inlineStr"/>
-      <c r="Y34" s="10" t="inlineStr"/>
-      <c r="Z34" s="10" t="inlineStr"/>
+          <t>13043-1899</t>
+        </is>
+      </c>
+      <c r="I34" s="5" t="inlineStr">
+        <is>
+          <t>SON566</t>
+        </is>
+      </c>
+      <c r="J34" s="11" t="n">
+        <v>44592.71537037037</v>
+      </c>
+      <c r="K34" s="11" t="n">
+        <v>44592.71540509259</v>
+      </c>
+      <c r="L34" s="11" t="n">
+        <v>44592.71572916667</v>
+      </c>
+      <c r="M34" s="11" t="n">
+        <v>44592.7529050926</v>
+      </c>
+      <c r="N34" s="11" t="n">
+        <v>44592.7531712963</v>
+      </c>
+      <c r="O34" s="11" t="n">
+        <v>44592.81997685185</v>
+      </c>
+      <c r="P34" s="11" t="n">
+        <v>44592.82001157408</v>
+      </c>
+      <c r="Q34" s="11" t="n">
+        <v>44592.82003472222</v>
+      </c>
+      <c r="R34" s="11" t="n">
+        <v>44593.25921296296</v>
+      </c>
+      <c r="S34" s="11" t="n">
+        <v>44593.25924768519</v>
+      </c>
+      <c r="T34" s="11" t="n">
+        <v>44593.25928240741</v>
+      </c>
+      <c r="U34" s="10" t="n">
+        <v>0.0003587962962962963</v>
+      </c>
+      <c r="V34" s="10" t="n">
+        <v>0.03717592592592592</v>
+      </c>
+      <c r="W34" s="10" t="n">
+        <v>0.0002662037037037037</v>
+      </c>
+      <c r="X34" s="10" t="n">
+        <v>0.06680555555555556</v>
+      </c>
+      <c r="Y34" s="10" t="n">
+        <v>5.787037037037037e-05</v>
+      </c>
+      <c r="Z34" s="10" t="n">
+        <v>0.4391782407407407</v>
+      </c>
+      <c r="AA34" s="10" t="n">
+        <v>0.5439120370370371</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="8" t="n">
         <v>28</v>
       </c>
       <c r="B35" s="5" t="n">
-        <v>161362</v>
+        <v>161477</v>
       </c>
       <c r="C35" s="9" t="n">
-        <v>44592</v>
+        <v>44593</v>
       </c>
       <c r="D35" s="5" t="inlineStr">
         <is>
-          <t>FINALIZADA</t>
+          <t>ACEPTADA</t>
         </is>
       </c>
       <c r="E35" s="5" t="inlineStr">
         <is>
-          <t>FABIO ENRIQUE TORRES PANQUEBA</t>
+          <t>GILBERTO  VARGAS FERRO</t>
         </is>
       </c>
       <c r="F35" s="5" t="inlineStr">
         <is>
-          <t>1073503221</t>
+          <t>13526371</t>
         </is>
       </c>
       <c r="G35" s="5" t="inlineStr">
         <is>
-          <t>13043-1800</t>
+          <t>13043-1804</t>
         </is>
       </c>
       <c r="H35" s="5" t="inlineStr">
         <is>
-          <t>SON566</t>
-        </is>
-      </c>
-      <c r="I35" s="11" t="n">
-        <v>44592.9237037037</v>
+          <t>13043-1903</t>
+        </is>
+      </c>
+      <c r="I35" s="5" t="inlineStr">
+        <is>
+          <t>SMK294</t>
+        </is>
       </c>
       <c r="J35" s="11" t="n">
-        <v>44592.92373842592</v>
+        <v>44593.62864583333</v>
       </c>
       <c r="K35" s="11" t="n">
-        <v>44592.9240625</v>
+        <v>44593.62868055556</v>
       </c>
       <c r="L35" s="11" t="n">
-        <v>44592.96123842592</v>
-      </c>
-      <c r="M35" s="11" t="n">
-        <v>44592.96150462963</v>
-      </c>
-      <c r="N35" s="11" t="n">
-        <v>44593.02831018518</v>
-      </c>
-      <c r="O35" s="11" t="n">
-        <v>44593.0283449074</v>
-      </c>
-      <c r="P35" s="11" t="n">
-        <v>44593.02836805556</v>
-      </c>
-      <c r="Q35" s="11" t="n">
-        <v>44593.4675462963</v>
-      </c>
-      <c r="R35" s="11" t="n">
-        <v>44593.46758101852</v>
-      </c>
-      <c r="S35" s="11" t="n">
-        <v>44593.46761574074</v>
-      </c>
-      <c r="T35" s="10" t="n">
-        <v>0.0003587962962962963</v>
-      </c>
+        <v>44593.6291087963</v>
+      </c>
+      <c r="M35" s="5" t="inlineStr"/>
+      <c r="N35" s="5" t="inlineStr"/>
+      <c r="O35" s="5" t="inlineStr"/>
+      <c r="P35" s="5" t="inlineStr"/>
+      <c r="Q35" s="5" t="inlineStr"/>
+      <c r="R35" s="5" t="inlineStr"/>
+      <c r="S35" s="5" t="inlineStr"/>
+      <c r="T35" s="5" t="inlineStr"/>
       <c r="U35" s="10" t="n">
-        <v>0.03717592592592592</v>
-      </c>
-      <c r="V35" s="10" t="n">
-        <v>3.472222222222222e-05</v>
-      </c>
-      <c r="W35" s="10" t="n">
-        <v>3.472222222222222e-05</v>
-      </c>
-      <c r="X35" s="10" t="n">
-        <v>5.787037037037037e-05</v>
-      </c>
-      <c r="Y35" s="10" t="n">
-        <v>0.4391782407407407</v>
-      </c>
-      <c r="Z35" s="10" t="n">
-        <v>0.5439120370370371</v>
-      </c>
+        <v>0.000462962962962963</v>
+      </c>
+      <c r="V35" s="10" t="inlineStr"/>
+      <c r="W35" s="10" t="inlineStr"/>
+      <c r="X35" s="10" t="inlineStr"/>
+      <c r="Y35" s="10" t="inlineStr"/>
+      <c r="Z35" s="10" t="inlineStr"/>
+      <c r="AA35" s="10" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="8" t="n">
         <v>29</v>
       </c>
       <c r="B36" s="5" t="n">
-        <v>161477</v>
+        <v>161474</v>
       </c>
       <c r="C36" s="9" t="n">
         <v>44593</v>
@@ -2875,25 +3405,29 @@
       </c>
       <c r="E36" s="5" t="inlineStr">
         <is>
-          <t>GILBERTO  VARGAS FERRO</t>
+          <t>MAURICIO  PARDO MEDINA</t>
         </is>
       </c>
       <c r="F36" s="5" t="inlineStr">
         <is>
-          <t>13526371</t>
+          <t>79132547</t>
         </is>
       </c>
       <c r="G36" s="5" t="inlineStr">
         <is>
-          <t>13043-1804</t>
+          <t>13043-1803</t>
         </is>
       </c>
       <c r="H36" s="5" t="inlineStr">
         <is>
-          <t>SMK294</t>
-        </is>
-      </c>
-      <c r="I36" s="5" t="inlineStr"/>
+          <t>13043-1902</t>
+        </is>
+      </c>
+      <c r="I36" s="5" t="inlineStr">
+        <is>
+          <t>SNC949</t>
+        </is>
+      </c>
       <c r="J36" s="5" t="inlineStr"/>
       <c r="K36" s="5" t="inlineStr"/>
       <c r="L36" s="5" t="inlineStr"/>
@@ -2904,167 +3438,178 @@
       <c r="Q36" s="5" t="inlineStr"/>
       <c r="R36" s="5" t="inlineStr"/>
       <c r="S36" s="5" t="inlineStr"/>
-      <c r="T36" s="10" t="inlineStr"/>
+      <c r="T36" s="5" t="inlineStr"/>
       <c r="U36" s="10" t="inlineStr"/>
       <c r="V36" s="10" t="inlineStr"/>
       <c r="W36" s="10" t="inlineStr"/>
       <c r="X36" s="10" t="inlineStr"/>
       <c r="Y36" s="10" t="inlineStr"/>
       <c r="Z36" s="10" t="inlineStr"/>
+      <c r="AA36" s="10" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="8" t="n">
         <v>30</v>
       </c>
       <c r="B37" s="5" t="n">
-        <v>161474</v>
+        <v>161478</v>
       </c>
       <c r="C37" s="9" t="n">
         <v>44593</v>
       </c>
       <c r="D37" s="5" t="inlineStr">
         <is>
-          <t>GENERADA</t>
+          <t>FINALIZADA</t>
         </is>
       </c>
       <c r="E37" s="5" t="inlineStr">
         <is>
-          <t>MAURICIO  PARDO MEDINA</t>
+          <t>FABIO ENRIQUE TORRES PANQUEBA</t>
         </is>
       </c>
       <c r="F37" s="5" t="inlineStr">
         <is>
-          <t>79132547</t>
+          <t>1073503221</t>
         </is>
       </c>
       <c r="G37" s="5" t="inlineStr">
         <is>
-          <t>13043-1803</t>
+          <t>13075-7074</t>
         </is>
       </c>
       <c r="H37" s="5" t="inlineStr">
         <is>
-          <t>SNC949</t>
-        </is>
-      </c>
-      <c r="I37" s="5" t="inlineStr"/>
-      <c r="J37" s="5" t="inlineStr"/>
-      <c r="K37" s="5" t="inlineStr"/>
-      <c r="L37" s="5" t="inlineStr"/>
-      <c r="M37" s="5" t="inlineStr"/>
-      <c r="N37" s="5" t="inlineStr"/>
-      <c r="O37" s="5" t="inlineStr"/>
-      <c r="P37" s="5" t="inlineStr"/>
-      <c r="Q37" s="5" t="inlineStr"/>
-      <c r="R37" s="5" t="inlineStr"/>
-      <c r="S37" s="5" t="inlineStr"/>
-      <c r="T37" s="10" t="inlineStr"/>
-      <c r="U37" s="10" t="inlineStr"/>
-      <c r="V37" s="10" t="inlineStr"/>
-      <c r="W37" s="10" t="inlineStr"/>
-      <c r="X37" s="10" t="inlineStr"/>
-      <c r="Y37" s="10" t="inlineStr"/>
-      <c r="Z37" s="10" t="inlineStr"/>
+          <t>13075-7263</t>
+        </is>
+      </c>
+      <c r="I37" s="5" t="inlineStr">
+        <is>
+          <t>SON566</t>
+        </is>
+      </c>
+      <c r="J37" s="11" t="n">
+        <v>44594.28001157408</v>
+      </c>
+      <c r="K37" s="11" t="n">
+        <v>44594.2800462963</v>
+      </c>
+      <c r="L37" s="11" t="n">
+        <v>44594.28075231481</v>
+      </c>
+      <c r="M37" s="11" t="n">
+        <v>44594.28253472222</v>
+      </c>
+      <c r="N37" s="11" t="n">
+        <v>44594.28270833333</v>
+      </c>
+      <c r="O37" s="11" t="n">
+        <v>44594.42641203704</v>
+      </c>
+      <c r="P37" s="11" t="n">
+        <v>44594.42645833334</v>
+      </c>
+      <c r="Q37" s="11" t="n">
+        <v>44594.42649305556</v>
+      </c>
+      <c r="R37" s="11" t="n">
+        <v>44594.48300925926</v>
+      </c>
+      <c r="S37" s="11" t="n">
+        <v>44594.48304398148</v>
+      </c>
+      <c r="T37" s="11" t="n">
+        <v>44594.48307870371</v>
+      </c>
+      <c r="U37" s="10" t="n">
+        <v>0.0007407407407407407</v>
+      </c>
+      <c r="V37" s="10" t="n">
+        <v>0.001782407407407407</v>
+      </c>
+      <c r="W37" s="10" t="n">
+        <v>0.0001736111111111111</v>
+      </c>
+      <c r="X37" s="10" t="n">
+        <v>0.1437037037037037</v>
+      </c>
+      <c r="Y37" s="10" t="n">
+        <v>8.101851851851852e-05</v>
+      </c>
+      <c r="Z37" s="10" t="n">
+        <v>0.0565162037037037</v>
+      </c>
+      <c r="AA37" s="10" t="n">
+        <v>0.2030671296296296</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="8" t="n">
         <v>31</v>
       </c>
       <c r="B38" s="5" t="n">
-        <v>161478</v>
+        <v>161479</v>
       </c>
       <c r="C38" s="9" t="n">
         <v>44593</v>
       </c>
       <c r="D38" s="5" t="inlineStr">
         <is>
-          <t>FINALIZADA</t>
+          <t>NOTIFICADA</t>
         </is>
       </c>
       <c r="E38" s="5" t="inlineStr">
         <is>
-          <t>FABIO ENRIQUE TORRES PANQUEBA</t>
+          <t>ELKIN FABIAN GONZALEZ BUSTOS</t>
         </is>
       </c>
       <c r="F38" s="5" t="inlineStr">
         <is>
-          <t>1073503221</t>
+          <t>1071165330</t>
         </is>
       </c>
       <c r="G38" s="5" t="inlineStr">
         <is>
-          <t>13075-7074</t>
+          <t>13075-7075</t>
         </is>
       </c>
       <c r="H38" s="5" t="inlineStr">
         <is>
-          <t>SON566</t>
-        </is>
-      </c>
-      <c r="I38" s="11" t="n">
-        <v>44594.4883449074</v>
-      </c>
-      <c r="J38" s="11" t="n">
-        <v>44594.48837962963</v>
-      </c>
-      <c r="K38" s="11" t="n">
-        <v>44594.48908564815</v>
-      </c>
-      <c r="L38" s="11" t="n">
-        <v>44594.49086805555</v>
-      </c>
-      <c r="M38" s="11" t="n">
-        <v>44594.49104166667</v>
-      </c>
-      <c r="N38" s="11" t="n">
-        <v>44594.63474537037</v>
-      </c>
-      <c r="O38" s="11" t="n">
-        <v>44594.63479166666</v>
-      </c>
-      <c r="P38" s="11" t="n">
-        <v>44594.63482638889</v>
-      </c>
-      <c r="Q38" s="11" t="n">
-        <v>44594.6913425926</v>
-      </c>
-      <c r="R38" s="11" t="n">
-        <v>44594.69137731481</v>
-      </c>
-      <c r="S38" s="11" t="n">
-        <v>44594.69141203703</v>
-      </c>
-      <c r="T38" s="10" t="n">
-        <v>0.0007407407407407407</v>
-      </c>
-      <c r="U38" s="10" t="n">
-        <v>0.001782407407407407</v>
-      </c>
-      <c r="V38" s="10" t="n">
-        <v>3.472222222222222e-05</v>
-      </c>
-      <c r="W38" s="10" t="n">
-        <v>3.472222222222222e-05</v>
-      </c>
-      <c r="X38" s="10" t="n">
-        <v>8.101851851851852e-05</v>
-      </c>
-      <c r="Y38" s="10" t="n">
-        <v>0.0565162037037037</v>
-      </c>
-      <c r="Z38" s="10" t="n">
-        <v>0.2030671296296296</v>
-      </c>
+          <t>13075-7259</t>
+        </is>
+      </c>
+      <c r="I38" s="5" t="inlineStr">
+        <is>
+          <t>SJQ652</t>
+        </is>
+      </c>
+      <c r="J38" s="5" t="inlineStr"/>
+      <c r="K38" s="5" t="inlineStr"/>
+      <c r="L38" s="5" t="inlineStr"/>
+      <c r="M38" s="5" t="inlineStr"/>
+      <c r="N38" s="5" t="inlineStr"/>
+      <c r="O38" s="5" t="inlineStr"/>
+      <c r="P38" s="5" t="inlineStr"/>
+      <c r="Q38" s="5" t="inlineStr"/>
+      <c r="R38" s="5" t="inlineStr"/>
+      <c r="S38" s="5" t="inlineStr"/>
+      <c r="T38" s="5" t="inlineStr"/>
+      <c r="U38" s="10" t="inlineStr"/>
+      <c r="V38" s="10" t="inlineStr"/>
+      <c r="W38" s="10" t="inlineStr"/>
+      <c r="X38" s="10" t="inlineStr"/>
+      <c r="Y38" s="10" t="inlineStr"/>
+      <c r="Z38" s="10" t="inlineStr"/>
+      <c r="AA38" s="10" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="8" t="n">
         <v>32</v>
       </c>
       <c r="B39" s="5" t="n">
-        <v>161479</v>
+        <v>161572</v>
       </c>
       <c r="C39" s="9" t="n">
-        <v>44593</v>
+        <v>44594</v>
       </c>
       <c r="D39" s="5" t="inlineStr">
         <is>
@@ -3073,25 +3618,29 @@
       </c>
       <c r="E39" s="5" t="inlineStr">
         <is>
-          <t>ELKIN FABIAN GONZALEZ BUSTOS</t>
+          <t>CIRO ANTONIO CAMACHO FERRO</t>
         </is>
       </c>
       <c r="F39" s="5" t="inlineStr">
         <is>
-          <t>1071165330</t>
+          <t>13526162</t>
         </is>
       </c>
       <c r="G39" s="5" t="inlineStr">
         <is>
-          <t>13075-7075</t>
+          <t>13075-7090</t>
         </is>
       </c>
       <c r="H39" s="5" t="inlineStr">
         <is>
-          <t>SJQ652</t>
-        </is>
-      </c>
-      <c r="I39" s="5" t="inlineStr"/>
+          <t>13075-7278</t>
+        </is>
+      </c>
+      <c r="I39" s="5" t="inlineStr">
+        <is>
+          <t>SUC236</t>
+        </is>
+      </c>
       <c r="J39" s="5" t="inlineStr"/>
       <c r="K39" s="5" t="inlineStr"/>
       <c r="L39" s="5" t="inlineStr"/>
@@ -3102,20 +3651,21 @@
       <c r="Q39" s="5" t="inlineStr"/>
       <c r="R39" s="5" t="inlineStr"/>
       <c r="S39" s="5" t="inlineStr"/>
-      <c r="T39" s="10" t="inlineStr"/>
+      <c r="T39" s="5" t="inlineStr"/>
       <c r="U39" s="10" t="inlineStr"/>
       <c r="V39" s="10" t="inlineStr"/>
       <c r="W39" s="10" t="inlineStr"/>
       <c r="X39" s="10" t="inlineStr"/>
       <c r="Y39" s="10" t="inlineStr"/>
       <c r="Z39" s="10" t="inlineStr"/>
+      <c r="AA39" s="10" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="8" t="n">
         <v>33</v>
       </c>
       <c r="B40" s="5" t="n">
-        <v>161572</v>
+        <v>161603</v>
       </c>
       <c r="C40" s="9" t="n">
         <v>44594</v>
@@ -3137,15 +3687,19 @@
       </c>
       <c r="G40" s="5" t="inlineStr">
         <is>
-          <t>13075-7090</t>
+          <t>13043-1808</t>
         </is>
       </c>
       <c r="H40" s="5" t="inlineStr">
         <is>
+          <t>13043-1907</t>
+        </is>
+      </c>
+      <c r="I40" s="5" t="inlineStr">
+        <is>
           <t>SUC236</t>
         </is>
       </c>
-      <c r="I40" s="5" t="inlineStr"/>
       <c r="J40" s="5" t="inlineStr"/>
       <c r="K40" s="5" t="inlineStr"/>
       <c r="L40" s="5" t="inlineStr"/>
@@ -3156,20 +3710,21 @@
       <c r="Q40" s="5" t="inlineStr"/>
       <c r="R40" s="5" t="inlineStr"/>
       <c r="S40" s="5" t="inlineStr"/>
-      <c r="T40" s="10" t="inlineStr"/>
+      <c r="T40" s="5" t="inlineStr"/>
       <c r="U40" s="10" t="inlineStr"/>
       <c r="V40" s="10" t="inlineStr"/>
       <c r="W40" s="10" t="inlineStr"/>
       <c r="X40" s="10" t="inlineStr"/>
       <c r="Y40" s="10" t="inlineStr"/>
       <c r="Z40" s="10" t="inlineStr"/>
+      <c r="AA40" s="10" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="8" t="n">
         <v>34</v>
       </c>
       <c r="B41" s="5" t="n">
-        <v>161603</v>
+        <v>161590</v>
       </c>
       <c r="C41" s="9" t="n">
         <v>44594</v>
@@ -3181,25 +3736,29 @@
       </c>
       <c r="E41" s="5" t="inlineStr">
         <is>
-          <t>CIRO ANTONIO CAMACHO FERRO</t>
+          <t>RICARDO ANDRES RODRIGUEZ ALDANA</t>
         </is>
       </c>
       <c r="F41" s="5" t="inlineStr">
         <is>
-          <t>13526162</t>
+          <t>1016058400</t>
         </is>
       </c>
       <c r="G41" s="5" t="inlineStr">
         <is>
-          <t>13043-1808</t>
+          <t>13039-27</t>
         </is>
       </c>
       <c r="H41" s="5" t="inlineStr">
         <is>
-          <t>SUC236</t>
-        </is>
-      </c>
-      <c r="I41" s="5" t="inlineStr"/>
+          <t>13039-33</t>
+        </is>
+      </c>
+      <c r="I41" s="5" t="inlineStr">
+        <is>
+          <t>THY168</t>
+        </is>
+      </c>
       <c r="J41" s="5" t="inlineStr"/>
       <c r="K41" s="5" t="inlineStr"/>
       <c r="L41" s="5" t="inlineStr"/>
@@ -3210,180 +3769,209 @@
       <c r="Q41" s="5" t="inlineStr"/>
       <c r="R41" s="5" t="inlineStr"/>
       <c r="S41" s="5" t="inlineStr"/>
-      <c r="T41" s="10" t="inlineStr"/>
+      <c r="T41" s="5" t="inlineStr"/>
       <c r="U41" s="10" t="inlineStr"/>
       <c r="V41" s="10" t="inlineStr"/>
       <c r="W41" s="10" t="inlineStr"/>
       <c r="X41" s="10" t="inlineStr"/>
       <c r="Y41" s="10" t="inlineStr"/>
       <c r="Z41" s="10" t="inlineStr"/>
+      <c r="AA41" s="10" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="8" t="n">
         <v>35</v>
       </c>
       <c r="B42" s="5" t="n">
-        <v>161590</v>
+        <v>161601</v>
       </c>
       <c r="C42" s="9" t="n">
         <v>44594</v>
       </c>
       <c r="D42" s="5" t="inlineStr">
         <is>
-          <t>GENERADA</t>
+          <t>FINALIZADA</t>
         </is>
       </c>
       <c r="E42" s="5" t="inlineStr">
         <is>
-          <t>RICARDO ANDRES RODRIGUEZ ALDANA</t>
+          <t>FABIO ENRIQUE TORRES PANQUEBA</t>
         </is>
       </c>
       <c r="F42" s="5" t="inlineStr">
         <is>
-          <t>1016058400</t>
+          <t>1073503221</t>
         </is>
       </c>
       <c r="G42" s="5" t="inlineStr">
         <is>
-          <t>13039-27</t>
+          <t>13043-1807</t>
         </is>
       </c>
       <c r="H42" s="5" t="inlineStr">
         <is>
-          <t>THY168</t>
-        </is>
-      </c>
-      <c r="I42" s="5" t="inlineStr"/>
-      <c r="J42" s="5" t="inlineStr"/>
-      <c r="K42" s="5" t="inlineStr"/>
-      <c r="L42" s="5" t="inlineStr"/>
-      <c r="M42" s="5" t="inlineStr"/>
-      <c r="N42" s="5" t="inlineStr"/>
-      <c r="O42" s="5" t="inlineStr"/>
-      <c r="P42" s="5" t="inlineStr"/>
-      <c r="Q42" s="5" t="inlineStr"/>
-      <c r="R42" s="5" t="inlineStr"/>
-      <c r="S42" s="5" t="inlineStr"/>
-      <c r="T42" s="10" t="inlineStr"/>
-      <c r="U42" s="10" t="inlineStr"/>
-      <c r="V42" s="10" t="inlineStr"/>
-      <c r="W42" s="10" t="inlineStr"/>
-      <c r="X42" s="10" t="inlineStr"/>
-      <c r="Y42" s="10" t="inlineStr"/>
-      <c r="Z42" s="10" t="inlineStr"/>
+          <t>13043-1906</t>
+        </is>
+      </c>
+      <c r="I42" s="5" t="inlineStr">
+        <is>
+          <t>SON566</t>
+        </is>
+      </c>
+      <c r="J42" s="11" t="n">
+        <v>44594.57010416667</v>
+      </c>
+      <c r="K42" s="11" t="n">
+        <v>44594.57013888889</v>
+      </c>
+      <c r="L42" s="11" t="n">
+        <v>44594.57028935185</v>
+      </c>
+      <c r="M42" s="11" t="n">
+        <v>44594.57039351852</v>
+      </c>
+      <c r="N42" s="11" t="n">
+        <v>44594.60534722222</v>
+      </c>
+      <c r="O42" s="11" t="n">
+        <v>44594.60564814815</v>
+      </c>
+      <c r="P42" s="11" t="n">
+        <v>44594.62943287037</v>
+      </c>
+      <c r="Q42" s="11" t="n">
+        <v>44594.68984953704</v>
+      </c>
+      <c r="R42" s="11" t="n">
+        <v>44595.36434027777</v>
+      </c>
+      <c r="S42" s="11" t="n">
+        <v>44595.36436342593</v>
+      </c>
+      <c r="T42" s="11" t="n">
+        <v>44595.36439814815</v>
+      </c>
+      <c r="U42" s="10" t="n">
+        <v>0.0001851851851851852</v>
+      </c>
+      <c r="V42" s="10" t="n">
+        <v>0.0001041666666666667</v>
+      </c>
+      <c r="W42" s="10" t="n">
+        <v>0.0349537037037037</v>
+      </c>
+      <c r="X42" s="10" t="n">
+        <v>0.0003009259259259259</v>
+      </c>
+      <c r="Y42" s="10" t="n">
+        <v>0.0842013888888889</v>
+      </c>
+      <c r="Z42" s="10" t="n">
+        <v>0.6744907407407408</v>
+      </c>
+      <c r="AA42" s="10" t="n">
+        <v>0.7942939814814814</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="8" t="n">
         <v>36</v>
       </c>
       <c r="B43" s="5" t="n">
-        <v>161601</v>
+        <v>161803</v>
       </c>
       <c r="C43" s="9" t="n">
-        <v>44594</v>
+        <v>44595</v>
       </c>
       <c r="D43" s="5" t="inlineStr">
         <is>
-          <t>ACEPTADA</t>
+          <t>GENERADA</t>
         </is>
       </c>
       <c r="E43" s="5" t="inlineStr">
         <is>
-          <t>FABIO ENRIQUE TORRES PANQUEBA</t>
+          <t>GILBERTO  VARGAS FERRO</t>
         </is>
       </c>
       <c r="F43" s="5" t="inlineStr">
         <is>
-          <t>1073503221</t>
+          <t>13526371</t>
         </is>
       </c>
       <c r="G43" s="5" t="inlineStr">
         <is>
-          <t>13043-1807</t>
+          <t>13075-7119</t>
         </is>
       </c>
       <c r="H43" s="5" t="inlineStr">
         <is>
-          <t>SON566</t>
-        </is>
-      </c>
-      <c r="I43" s="11" t="n">
-        <v>44594.7784375</v>
-      </c>
-      <c r="J43" s="11" t="n">
-        <v>44594.77847222222</v>
-      </c>
-      <c r="K43" s="11" t="n">
-        <v>44594.77862268518</v>
-      </c>
-      <c r="L43" s="11" t="n">
-        <v>44594.77872685185</v>
-      </c>
-      <c r="M43" s="11" t="n">
-        <v>44594.81368055556</v>
-      </c>
-      <c r="N43" s="11" t="n">
-        <v>44594.81398148148</v>
-      </c>
-      <c r="O43" s="11" t="n">
-        <v>44594.8377662037</v>
-      </c>
-      <c r="P43" s="11" t="n">
-        <v>44594.89818287037</v>
-      </c>
+          <t>13075-7301</t>
+        </is>
+      </c>
+      <c r="I43" s="5" t="inlineStr">
+        <is>
+          <t>SKF030</t>
+        </is>
+      </c>
+      <c r="J43" s="5" t="inlineStr"/>
+      <c r="K43" s="5" t="inlineStr"/>
+      <c r="L43" s="5" t="inlineStr"/>
+      <c r="M43" s="5" t="inlineStr"/>
+      <c r="N43" s="5" t="inlineStr"/>
+      <c r="O43" s="5" t="inlineStr"/>
+      <c r="P43" s="5" t="inlineStr"/>
       <c r="Q43" s="5" t="inlineStr"/>
       <c r="R43" s="5" t="inlineStr"/>
       <c r="S43" s="5" t="inlineStr"/>
-      <c r="T43" s="10" t="n">
-        <v>0.0001851851851851852</v>
-      </c>
-      <c r="U43" s="10" t="n">
-        <v>0.0001041666666666667</v>
-      </c>
+      <c r="T43" s="5" t="inlineStr"/>
+      <c r="U43" s="10" t="inlineStr"/>
       <c r="V43" s="10" t="inlineStr"/>
       <c r="W43" s="10" t="inlineStr"/>
-      <c r="X43" s="10" t="n">
-        <v>0.0842013888888889</v>
-      </c>
+      <c r="X43" s="10" t="inlineStr"/>
       <c r="Y43" s="10" t="inlineStr"/>
       <c r="Z43" s="10" t="inlineStr"/>
+      <c r="AA43" s="10" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="8" t="n">
         <v>37</v>
       </c>
       <c r="B44" s="5" t="n">
-        <v>161606</v>
+        <v>161804</v>
       </c>
       <c r="C44" s="9" t="n">
-        <v>44594</v>
+        <v>44595</v>
       </c>
       <c r="D44" s="5" t="inlineStr">
         <is>
-          <t>NOTIFICADA</t>
+          <t>GENERADA</t>
         </is>
       </c>
       <c r="E44" s="5" t="inlineStr">
         <is>
-          <t>WILSON LEONIDAS GUTIERREZ BARON</t>
+          <t>GILBERTO  VARGAS FERRO</t>
         </is>
       </c>
       <c r="F44" s="5" t="inlineStr">
         <is>
-          <t>79987585</t>
+          <t>13526371</t>
         </is>
       </c>
       <c r="G44" s="5" t="inlineStr">
         <is>
-          <t>13075-7091</t>
+          <t>13075-7120</t>
         </is>
       </c>
       <c r="H44" s="5" t="inlineStr">
         <is>
-          <t>SMK294</t>
-        </is>
-      </c>
-      <c r="I44" s="5" t="inlineStr"/>
+          <t>13075-7302</t>
+        </is>
+      </c>
+      <c r="I44" s="5" t="inlineStr">
+        <is>
+          <t>SKF030</t>
+        </is>
+      </c>
       <c r="J44" s="5" t="inlineStr"/>
       <c r="K44" s="5" t="inlineStr"/>
       <c r="L44" s="5" t="inlineStr"/>
@@ -3394,67 +3982,1207 @@
       <c r="Q44" s="5" t="inlineStr"/>
       <c r="R44" s="5" t="inlineStr"/>
       <c r="S44" s="5" t="inlineStr"/>
-      <c r="T44" s="10" t="inlineStr"/>
+      <c r="T44" s="5" t="inlineStr"/>
       <c r="U44" s="10" t="inlineStr"/>
       <c r="V44" s="10" t="inlineStr"/>
       <c r="W44" s="10" t="inlineStr"/>
       <c r="X44" s="10" t="inlineStr"/>
       <c r="Y44" s="10" t="inlineStr"/>
       <c r="Z44" s="10" t="inlineStr"/>
+      <c r="AA44" s="10" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="8" t="n">
         <v>38</v>
       </c>
       <c r="B45" s="5" t="n">
-        <v>161607</v>
+        <v>161805</v>
       </c>
       <c r="C45" s="9" t="n">
-        <v>44594</v>
+        <v>44595</v>
       </c>
       <c r="D45" s="5" t="inlineStr">
         <is>
-          <t>NOTIFICADA</t>
+          <t>ACEPTADA</t>
         </is>
       </c>
       <c r="E45" s="5" t="inlineStr">
         <is>
-          <t>WILSON LEONIDAS GUTIERREZ BARON</t>
+          <t>ELKIN FABIAN GONZALEZ BUSTOS</t>
         </is>
       </c>
       <c r="F45" s="5" t="inlineStr">
         <is>
-          <t>79987585</t>
+          <t>1071165330</t>
         </is>
       </c>
       <c r="G45" s="5" t="inlineStr">
         <is>
-          <t>13075-7092</t>
+          <t>13075-7121</t>
         </is>
       </c>
       <c r="H45" s="5" t="inlineStr">
         <is>
-          <t>SMK294</t>
-        </is>
-      </c>
-      <c r="I45" s="5" t="inlineStr"/>
-      <c r="J45" s="5" t="inlineStr"/>
-      <c r="K45" s="5" t="inlineStr"/>
-      <c r="L45" s="5" t="inlineStr"/>
-      <c r="M45" s="5" t="inlineStr"/>
-      <c r="N45" s="5" t="inlineStr"/>
-      <c r="O45" s="5" t="inlineStr"/>
+          <t>13075-7297</t>
+        </is>
+      </c>
+      <c r="I45" s="5" t="inlineStr">
+        <is>
+          <t>SJQ652</t>
+        </is>
+      </c>
+      <c r="J45" s="11" t="n">
+        <v>44596.27704861111</v>
+      </c>
+      <c r="K45" s="11" t="n">
+        <v>44596.27711805556</v>
+      </c>
+      <c r="L45" s="11" t="n">
+        <v>44596.32012731482</v>
+      </c>
+      <c r="M45" s="11" t="n">
+        <v>44596.34888888889</v>
+      </c>
+      <c r="N45" s="11" t="n">
+        <v>44596.35957175926</v>
+      </c>
+      <c r="O45" s="11" t="n">
+        <v>44596.39363425926</v>
+      </c>
       <c r="P45" s="5" t="inlineStr"/>
       <c r="Q45" s="5" t="inlineStr"/>
       <c r="R45" s="5" t="inlineStr"/>
       <c r="S45" s="5" t="inlineStr"/>
-      <c r="T45" s="10" t="inlineStr"/>
-      <c r="U45" s="10" t="inlineStr"/>
-      <c r="V45" s="10" t="inlineStr"/>
-      <c r="W45" s="10" t="inlineStr"/>
-      <c r="X45" s="10" t="inlineStr"/>
+      <c r="T45" s="5" t="inlineStr"/>
+      <c r="U45" s="10" t="n">
+        <v>0.0430787037037037</v>
+      </c>
+      <c r="V45" s="10" t="n">
+        <v>0.02876157407407407</v>
+      </c>
+      <c r="W45" s="10" t="n">
+        <v>0.01068287037037037</v>
+      </c>
+      <c r="X45" s="10" t="n">
+        <v>0.0340625</v>
+      </c>
       <c r="Y45" s="10" t="inlineStr"/>
       <c r="Z45" s="10" t="inlineStr"/>
+      <c r="AA45" s="10" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="8" t="n">
+        <v>39</v>
+      </c>
+      <c r="B46" s="5" t="n">
+        <v>161607</v>
+      </c>
+      <c r="C46" s="9" t="n">
+        <v>44594</v>
+      </c>
+      <c r="D46" s="5" t="inlineStr">
+        <is>
+          <t>FINALIZADA</t>
+        </is>
+      </c>
+      <c r="E46" s="5" t="inlineStr">
+        <is>
+          <t>WILSON LEONIDAS GUTIERREZ BARON</t>
+        </is>
+      </c>
+      <c r="F46" s="5" t="inlineStr">
+        <is>
+          <t>79987585</t>
+        </is>
+      </c>
+      <c r="G46" s="5" t="inlineStr">
+        <is>
+          <t>13075-7092</t>
+        </is>
+      </c>
+      <c r="H46" s="5" t="inlineStr">
+        <is>
+          <t>13075-7291</t>
+        </is>
+      </c>
+      <c r="I46" s="5" t="inlineStr">
+        <is>
+          <t>SMK294</t>
+        </is>
+      </c>
+      <c r="J46" s="11" t="n">
+        <v>44595.10188657408</v>
+      </c>
+      <c r="K46" s="11" t="n">
+        <v>44595.10600694444</v>
+      </c>
+      <c r="L46" s="11" t="n">
+        <v>44595.11277777778</v>
+      </c>
+      <c r="M46" s="11" t="n">
+        <v>44595.13903935185</v>
+      </c>
+      <c r="N46" s="11" t="n">
+        <v>44595.14791666667</v>
+      </c>
+      <c r="O46" s="11" t="n">
+        <v>44595.18697916667</v>
+      </c>
+      <c r="P46" s="11" t="n">
+        <v>44595.18884259259</v>
+      </c>
+      <c r="Q46" s="11" t="n">
+        <v>44595.46896990741</v>
+      </c>
+      <c r="R46" s="11" t="n">
+        <v>44595.46922453704</v>
+      </c>
+      <c r="S46" s="11" t="n">
+        <v>44595.46925925926</v>
+      </c>
+      <c r="T46" s="11" t="n">
+        <v>44595.46930555555</v>
+      </c>
+      <c r="U46" s="10" t="n">
+        <v>0.0108912037037037</v>
+      </c>
+      <c r="V46" s="10" t="n">
+        <v>0.02626157407407407</v>
+      </c>
+      <c r="W46" s="10" t="n">
+        <v>0.008877314814814815</v>
+      </c>
+      <c r="X46" s="10" t="n">
+        <v>0.0390625</v>
+      </c>
+      <c r="Y46" s="10" t="n">
+        <v>0.2819907407407408</v>
+      </c>
+      <c r="Z46" s="10" t="n">
+        <v>0.0002546296296296296</v>
+      </c>
+      <c r="AA46" s="10" t="n">
+        <v>0.3674189814814815</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="8" t="n">
+        <v>40</v>
+      </c>
+      <c r="B47" s="5" t="n">
+        <v>161806</v>
+      </c>
+      <c r="C47" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D47" s="5" t="inlineStr">
+        <is>
+          <t>NOTIFICADA</t>
+        </is>
+      </c>
+      <c r="E47" s="5" t="inlineStr">
+        <is>
+          <t>ELKIN FABIAN GONZALEZ BUSTOS</t>
+        </is>
+      </c>
+      <c r="F47" s="5" t="inlineStr">
+        <is>
+          <t>1071165330</t>
+        </is>
+      </c>
+      <c r="G47" s="5" t="inlineStr">
+        <is>
+          <t>13075-7122</t>
+        </is>
+      </c>
+      <c r="H47" s="5" t="inlineStr">
+        <is>
+          <t>13075-7298</t>
+        </is>
+      </c>
+      <c r="I47" s="5" t="inlineStr">
+        <is>
+          <t>SJQ652</t>
+        </is>
+      </c>
+      <c r="J47" s="5" t="inlineStr"/>
+      <c r="K47" s="5" t="inlineStr"/>
+      <c r="L47" s="5" t="inlineStr"/>
+      <c r="M47" s="5" t="inlineStr"/>
+      <c r="N47" s="5" t="inlineStr"/>
+      <c r="O47" s="5" t="inlineStr"/>
+      <c r="P47" s="5" t="inlineStr"/>
+      <c r="Q47" s="5" t="inlineStr"/>
+      <c r="R47" s="5" t="inlineStr"/>
+      <c r="S47" s="5" t="inlineStr"/>
+      <c r="T47" s="5" t="inlineStr"/>
+      <c r="U47" s="10" t="inlineStr"/>
+      <c r="V47" s="10" t="inlineStr"/>
+      <c r="W47" s="10" t="inlineStr"/>
+      <c r="X47" s="10" t="inlineStr"/>
+      <c r="Y47" s="10" t="inlineStr"/>
+      <c r="Z47" s="10" t="inlineStr"/>
+      <c r="AA47" s="10" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="8" t="n">
+        <v>41</v>
+      </c>
+      <c r="B48" s="5" t="n">
+        <v>161807</v>
+      </c>
+      <c r="C48" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D48" s="5" t="inlineStr">
+        <is>
+          <t>NOTIFICADA</t>
+        </is>
+      </c>
+      <c r="E48" s="5" t="inlineStr">
+        <is>
+          <t>ELKIN FABIAN GONZALEZ BUSTOS</t>
+        </is>
+      </c>
+      <c r="F48" s="5" t="inlineStr">
+        <is>
+          <t>1071165330</t>
+        </is>
+      </c>
+      <c r="G48" s="5" t="inlineStr">
+        <is>
+          <t>13075-7123</t>
+        </is>
+      </c>
+      <c r="H48" s="5" t="inlineStr">
+        <is>
+          <t>13075-7300</t>
+        </is>
+      </c>
+      <c r="I48" s="5" t="inlineStr">
+        <is>
+          <t>SJQ652</t>
+        </is>
+      </c>
+      <c r="J48" s="5" t="inlineStr"/>
+      <c r="K48" s="5" t="inlineStr"/>
+      <c r="L48" s="5" t="inlineStr"/>
+      <c r="M48" s="5" t="inlineStr"/>
+      <c r="N48" s="5" t="inlineStr"/>
+      <c r="O48" s="5" t="inlineStr"/>
+      <c r="P48" s="5" t="inlineStr"/>
+      <c r="Q48" s="5" t="inlineStr"/>
+      <c r="R48" s="5" t="inlineStr"/>
+      <c r="S48" s="5" t="inlineStr"/>
+      <c r="T48" s="5" t="inlineStr"/>
+      <c r="U48" s="10" t="inlineStr"/>
+      <c r="V48" s="10" t="inlineStr"/>
+      <c r="W48" s="10" t="inlineStr"/>
+      <c r="X48" s="10" t="inlineStr"/>
+      <c r="Y48" s="10" t="inlineStr"/>
+      <c r="Z48" s="10" t="inlineStr"/>
+      <c r="AA48" s="10" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="8" t="n">
+        <v>42</v>
+      </c>
+      <c r="B49" s="5" t="n">
+        <v>161959</v>
+      </c>
+      <c r="C49" s="9" t="n">
+        <v>44596</v>
+      </c>
+      <c r="D49" s="5" t="inlineStr">
+        <is>
+          <t>GENERADA</t>
+        </is>
+      </c>
+      <c r="E49" s="5" t="inlineStr">
+        <is>
+          <t>FABIO ENRIQUE TORRES PANQUEBA</t>
+        </is>
+      </c>
+      <c r="F49" s="5" t="inlineStr">
+        <is>
+          <t>1073503221</t>
+        </is>
+      </c>
+      <c r="G49" s="5" t="inlineStr">
+        <is>
+          <t>13043-1812</t>
+        </is>
+      </c>
+      <c r="H49" s="5" t="inlineStr">
+        <is>
+          <t>13043-1911</t>
+        </is>
+      </c>
+      <c r="I49" s="5" t="inlineStr">
+        <is>
+          <t>SON566</t>
+        </is>
+      </c>
+      <c r="J49" s="5" t="inlineStr"/>
+      <c r="K49" s="5" t="inlineStr"/>
+      <c r="L49" s="5" t="inlineStr"/>
+      <c r="M49" s="5" t="inlineStr"/>
+      <c r="N49" s="5" t="inlineStr"/>
+      <c r="O49" s="5" t="inlineStr"/>
+      <c r="P49" s="5" t="inlineStr"/>
+      <c r="Q49" s="5" t="inlineStr"/>
+      <c r="R49" s="5" t="inlineStr"/>
+      <c r="S49" s="5" t="inlineStr"/>
+      <c r="T49" s="5" t="inlineStr"/>
+      <c r="U49" s="10" t="inlineStr"/>
+      <c r="V49" s="10" t="inlineStr"/>
+      <c r="W49" s="10" t="inlineStr"/>
+      <c r="X49" s="10" t="inlineStr"/>
+      <c r="Y49" s="10" t="inlineStr"/>
+      <c r="Z49" s="10" t="inlineStr"/>
+      <c r="AA49" s="10" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="8" t="n">
+        <v>43</v>
+      </c>
+      <c r="B50" s="5" t="n">
+        <v>161810</v>
+      </c>
+      <c r="C50" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D50" s="5" t="inlineStr">
+        <is>
+          <t>GENERADA</t>
+        </is>
+      </c>
+      <c r="E50" s="5" t="inlineStr">
+        <is>
+          <t>CIRO ANTONIO CAMACHO FERRO</t>
+        </is>
+      </c>
+      <c r="F50" s="5" t="inlineStr">
+        <is>
+          <t>13526162</t>
+        </is>
+      </c>
+      <c r="G50" s="5" t="inlineStr">
+        <is>
+          <t>13075-7124</t>
+        </is>
+      </c>
+      <c r="H50" s="5" t="inlineStr">
+        <is>
+          <t>13075-7299</t>
+        </is>
+      </c>
+      <c r="I50" s="5" t="inlineStr">
+        <is>
+          <t>SUC236</t>
+        </is>
+      </c>
+      <c r="J50" s="5" t="inlineStr"/>
+      <c r="K50" s="5" t="inlineStr"/>
+      <c r="L50" s="5" t="inlineStr"/>
+      <c r="M50" s="5" t="inlineStr"/>
+      <c r="N50" s="5" t="inlineStr"/>
+      <c r="O50" s="5" t="inlineStr"/>
+      <c r="P50" s="5" t="inlineStr"/>
+      <c r="Q50" s="5" t="inlineStr"/>
+      <c r="R50" s="5" t="inlineStr"/>
+      <c r="S50" s="5" t="inlineStr"/>
+      <c r="T50" s="5" t="inlineStr"/>
+      <c r="U50" s="10" t="inlineStr"/>
+      <c r="V50" s="10" t="inlineStr"/>
+      <c r="W50" s="10" t="inlineStr"/>
+      <c r="X50" s="10" t="inlineStr"/>
+      <c r="Y50" s="10" t="inlineStr"/>
+      <c r="Z50" s="10" t="inlineStr"/>
+      <c r="AA50" s="10" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="8" t="n">
+        <v>44</v>
+      </c>
+      <c r="B51" s="5" t="n">
+        <v>161783</v>
+      </c>
+      <c r="C51" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D51" s="5" t="inlineStr">
+        <is>
+          <t>FINALIZADA</t>
+        </is>
+      </c>
+      <c r="E51" s="5" t="inlineStr">
+        <is>
+          <t>ELKIN FABIAN GONZALEZ BUSTOS</t>
+        </is>
+      </c>
+      <c r="F51" s="5" t="inlineStr">
+        <is>
+          <t>1071165330</t>
+        </is>
+      </c>
+      <c r="G51" s="5" t="inlineStr">
+        <is>
+          <t>13075-7107</t>
+        </is>
+      </c>
+      <c r="H51" s="5" t="inlineStr">
+        <is>
+          <t>13075-7296</t>
+        </is>
+      </c>
+      <c r="I51" s="5" t="inlineStr">
+        <is>
+          <t>SJQ652</t>
+        </is>
+      </c>
+      <c r="J51" s="11" t="n">
+        <v>44595.71534722222</v>
+      </c>
+      <c r="K51" s="11" t="n">
+        <v>44595.71542824074</v>
+      </c>
+      <c r="L51" s="11" t="n">
+        <v>44595.72652777778</v>
+      </c>
+      <c r="M51" s="11" t="n">
+        <v>44595.84151620371</v>
+      </c>
+      <c r="N51" s="11" t="n">
+        <v>44595.84174768518</v>
+      </c>
+      <c r="O51" s="11" t="n">
+        <v>44595.8440625</v>
+      </c>
+      <c r="P51" s="11" t="n">
+        <v>44595.84418981482</v>
+      </c>
+      <c r="Q51" s="11" t="n">
+        <v>44596.24608796297</v>
+      </c>
+      <c r="R51" s="11" t="n">
+        <v>44596.24618055556</v>
+      </c>
+      <c r="S51" s="11" t="n">
+        <v>44596.2462962963</v>
+      </c>
+      <c r="T51" s="11" t="n">
+        <v>44596.32024305555</v>
+      </c>
+      <c r="U51" s="10" t="n">
+        <v>0.01118055555555555</v>
+      </c>
+      <c r="V51" s="10" t="n">
+        <v>0.1149884259259259</v>
+      </c>
+      <c r="W51" s="10" t="n">
+        <v>0.0002314814814814815</v>
+      </c>
+      <c r="X51" s="10" t="n">
+        <v>0.002314814814814815</v>
+      </c>
+      <c r="Y51" s="10" t="n">
+        <v>0.402025462962963</v>
+      </c>
+      <c r="Z51" s="10" t="n">
+        <v>9.259259259259259e-05</v>
+      </c>
+      <c r="AA51" s="10" t="n">
+        <v>0.6048958333333333</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="8" t="n">
+        <v>45</v>
+      </c>
+      <c r="B52" s="5" t="n">
+        <v>161361</v>
+      </c>
+      <c r="C52" s="9" t="n">
+        <v>44592</v>
+      </c>
+      <c r="D52" s="5" t="inlineStr">
+        <is>
+          <t>NOTIFICADA</t>
+        </is>
+      </c>
+      <c r="E52" s="5" t="inlineStr">
+        <is>
+          <t>ELKIN FABIAN GONZALEZ BUSTOS</t>
+        </is>
+      </c>
+      <c r="F52" s="5" t="inlineStr">
+        <is>
+          <t>1071165330</t>
+        </is>
+      </c>
+      <c r="G52" s="5" t="inlineStr">
+        <is>
+          <t>13075-7067</t>
+        </is>
+      </c>
+      <c r="H52" s="5" t="inlineStr">
+        <is>
+          <t>13075-7247</t>
+        </is>
+      </c>
+      <c r="I52" s="5" t="inlineStr">
+        <is>
+          <t>SJQ652</t>
+        </is>
+      </c>
+      <c r="J52" s="5" t="inlineStr"/>
+      <c r="K52" s="5" t="inlineStr"/>
+      <c r="L52" s="5" t="inlineStr"/>
+      <c r="M52" s="5" t="inlineStr"/>
+      <c r="N52" s="5" t="inlineStr"/>
+      <c r="O52" s="5" t="inlineStr"/>
+      <c r="P52" s="5" t="inlineStr"/>
+      <c r="Q52" s="5" t="inlineStr"/>
+      <c r="R52" s="5" t="inlineStr"/>
+      <c r="S52" s="5" t="inlineStr"/>
+      <c r="T52" s="5" t="inlineStr"/>
+      <c r="U52" s="10" t="inlineStr"/>
+      <c r="V52" s="10" t="inlineStr"/>
+      <c r="W52" s="10" t="inlineStr"/>
+      <c r="X52" s="10" t="inlineStr"/>
+      <c r="Y52" s="10" t="inlineStr"/>
+      <c r="Z52" s="10" t="inlineStr"/>
+      <c r="AA52" s="10" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="8" t="n">
+        <v>46</v>
+      </c>
+      <c r="B53" s="5" t="n">
+        <v>161765</v>
+      </c>
+      <c r="C53" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D53" s="5" t="inlineStr">
+        <is>
+          <t>GENERADA</t>
+        </is>
+      </c>
+      <c r="E53" s="5" t="inlineStr">
+        <is>
+          <t>GILBERTO  VARGAS FERRO</t>
+        </is>
+      </c>
+      <c r="F53" s="5" t="inlineStr">
+        <is>
+          <t>13526371</t>
+        </is>
+      </c>
+      <c r="G53" s="5" t="inlineStr">
+        <is>
+          <t>13075-7104</t>
+        </is>
+      </c>
+      <c r="H53" s="5" t="inlineStr">
+        <is>
+          <t>13075-7293</t>
+        </is>
+      </c>
+      <c r="I53" s="5" t="inlineStr">
+        <is>
+          <t>SKF030</t>
+        </is>
+      </c>
+      <c r="J53" s="5" t="inlineStr"/>
+      <c r="K53" s="5" t="inlineStr"/>
+      <c r="L53" s="5" t="inlineStr"/>
+      <c r="M53" s="5" t="inlineStr"/>
+      <c r="N53" s="5" t="inlineStr"/>
+      <c r="O53" s="5" t="inlineStr"/>
+      <c r="P53" s="5" t="inlineStr"/>
+      <c r="Q53" s="5" t="inlineStr"/>
+      <c r="R53" s="5" t="inlineStr"/>
+      <c r="S53" s="5" t="inlineStr"/>
+      <c r="T53" s="5" t="inlineStr"/>
+      <c r="U53" s="10" t="inlineStr"/>
+      <c r="V53" s="10" t="inlineStr"/>
+      <c r="W53" s="10" t="inlineStr"/>
+      <c r="X53" s="10" t="inlineStr"/>
+      <c r="Y53" s="10" t="inlineStr"/>
+      <c r="Z53" s="10" t="inlineStr"/>
+      <c r="AA53" s="10" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="8" t="n">
+        <v>47</v>
+      </c>
+      <c r="B54" s="5" t="n">
+        <v>161756</v>
+      </c>
+      <c r="C54" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D54" s="5" t="inlineStr">
+        <is>
+          <t>FINALIZADA</t>
+        </is>
+      </c>
+      <c r="E54" s="5" t="inlineStr">
+        <is>
+          <t>FABIO ENRIQUE TORRES PANQUEBA</t>
+        </is>
+      </c>
+      <c r="F54" s="5" t="inlineStr">
+        <is>
+          <t>1073503221</t>
+        </is>
+      </c>
+      <c r="G54" s="5" t="inlineStr">
+        <is>
+          <t>13075-7103</t>
+        </is>
+      </c>
+      <c r="H54" s="5" t="inlineStr">
+        <is>
+          <t>13075-7292</t>
+        </is>
+      </c>
+      <c r="I54" s="5" t="inlineStr">
+        <is>
+          <t>SON566</t>
+        </is>
+      </c>
+      <c r="J54" s="11" t="n">
+        <v>44595.54994212963</v>
+      </c>
+      <c r="K54" s="11" t="n">
+        <v>44595.54998842593</v>
+      </c>
+      <c r="L54" s="11" t="n">
+        <v>44595.55012731482</v>
+      </c>
+      <c r="M54" s="11" t="n">
+        <v>44595.55025462963</v>
+      </c>
+      <c r="N54" s="11" t="n">
+        <v>44595.55043981481</v>
+      </c>
+      <c r="O54" s="11" t="n">
+        <v>44595.55744212963</v>
+      </c>
+      <c r="P54" s="11" t="n">
+        <v>44595.55747685185</v>
+      </c>
+      <c r="Q54" s="11" t="n">
+        <v>44595.5575462963</v>
+      </c>
+      <c r="R54" s="11" t="n">
+        <v>44595.62320601852</v>
+      </c>
+      <c r="S54" s="11" t="n">
+        <v>44595.62328703704</v>
+      </c>
+      <c r="T54" s="11" t="n">
+        <v>44595.62336805555</v>
+      </c>
+      <c r="U54" s="10" t="n">
+        <v>0.0001851851851851852</v>
+      </c>
+      <c r="V54" s="10" t="n">
+        <v>0.0001273148148148148</v>
+      </c>
+      <c r="W54" s="10" t="n">
+        <v>0.0001851851851851852</v>
+      </c>
+      <c r="X54" s="10" t="n">
+        <v>0.007002314814814815</v>
+      </c>
+      <c r="Y54" s="10" t="n">
+        <v>0.0001041666666666667</v>
+      </c>
+      <c r="Z54" s="10" t="n">
+        <v>0.06565972222222222</v>
+      </c>
+      <c r="AA54" s="10" t="n">
+        <v>0.07342592592592592</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="8" t="n">
+        <v>48</v>
+      </c>
+      <c r="B55" s="5" t="n">
+        <v>161782</v>
+      </c>
+      <c r="C55" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D55" s="5" t="inlineStr">
+        <is>
+          <t>GENERADA</t>
+        </is>
+      </c>
+      <c r="E55" s="5" t="inlineStr">
+        <is>
+          <t>RICARDO ANDRES RODRIGUEZ ALDANA</t>
+        </is>
+      </c>
+      <c r="F55" s="5" t="inlineStr">
+        <is>
+          <t>1016058400</t>
+        </is>
+      </c>
+      <c r="G55" s="5" t="inlineStr">
+        <is>
+          <t>13043-1809</t>
+        </is>
+      </c>
+      <c r="H55" s="5" t="inlineStr">
+        <is>
+          <t>13043-1908</t>
+        </is>
+      </c>
+      <c r="I55" s="5" t="inlineStr">
+        <is>
+          <t>THY168</t>
+        </is>
+      </c>
+      <c r="J55" s="5" t="inlineStr"/>
+      <c r="K55" s="5" t="inlineStr"/>
+      <c r="L55" s="5" t="inlineStr"/>
+      <c r="M55" s="5" t="inlineStr"/>
+      <c r="N55" s="5" t="inlineStr"/>
+      <c r="O55" s="5" t="inlineStr"/>
+      <c r="P55" s="5" t="inlineStr"/>
+      <c r="Q55" s="5" t="inlineStr"/>
+      <c r="R55" s="5" t="inlineStr"/>
+      <c r="S55" s="5" t="inlineStr"/>
+      <c r="T55" s="5" t="inlineStr"/>
+      <c r="U55" s="10" t="inlineStr"/>
+      <c r="V55" s="10" t="inlineStr"/>
+      <c r="W55" s="10" t="inlineStr"/>
+      <c r="X55" s="10" t="inlineStr"/>
+      <c r="Y55" s="10" t="inlineStr"/>
+      <c r="Z55" s="10" t="inlineStr"/>
+      <c r="AA55" s="10" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="8" t="n">
+        <v>49</v>
+      </c>
+      <c r="B56" s="5" t="n">
+        <v>161798</v>
+      </c>
+      <c r="C56" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D56" s="5" t="inlineStr">
+        <is>
+          <t>ACEPTADA</t>
+        </is>
+      </c>
+      <c r="E56" s="5" t="inlineStr">
+        <is>
+          <t>WILSON LEONIDAS GUTIERREZ BARON</t>
+        </is>
+      </c>
+      <c r="F56" s="5" t="inlineStr">
+        <is>
+          <t>79987585</t>
+        </is>
+      </c>
+      <c r="G56" s="5" t="inlineStr">
+        <is>
+          <t>13075-7109</t>
+        </is>
+      </c>
+      <c r="H56" s="5" t="inlineStr">
+        <is>
+          <t>13075-7311</t>
+        </is>
+      </c>
+      <c r="I56" s="5" t="inlineStr">
+        <is>
+          <t>SMK294</t>
+        </is>
+      </c>
+      <c r="J56" s="11" t="n">
+        <v>44595.86876157407</v>
+      </c>
+      <c r="K56" s="11" t="n">
+        <v>44595.87297453704</v>
+      </c>
+      <c r="L56" s="11" t="n">
+        <v>44595.88337962963</v>
+      </c>
+      <c r="M56" s="11" t="n">
+        <v>44595.89582175926</v>
+      </c>
+      <c r="N56" s="11" t="n">
+        <v>44595.90458333334</v>
+      </c>
+      <c r="O56" s="11" t="n">
+        <v>44595.92751157407</v>
+      </c>
+      <c r="P56" s="11" t="n">
+        <v>44595.93023148148</v>
+      </c>
+      <c r="Q56" s="11" t="n">
+        <v>44595.93478009259</v>
+      </c>
+      <c r="R56" s="5" t="inlineStr"/>
+      <c r="S56" s="5" t="inlineStr"/>
+      <c r="T56" s="5" t="inlineStr"/>
+      <c r="U56" s="10" t="n">
+        <v>0.01461805555555556</v>
+      </c>
+      <c r="V56" s="10" t="n">
+        <v>0.01244212962962963</v>
+      </c>
+      <c r="W56" s="10" t="n">
+        <v>0.008761574074074074</v>
+      </c>
+      <c r="X56" s="10" t="n">
+        <v>0.02292824074074074</v>
+      </c>
+      <c r="Y56" s="10" t="n">
+        <v>0.007268518518518519</v>
+      </c>
+      <c r="Z56" s="10" t="inlineStr"/>
+      <c r="AA56" s="10" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="B57" s="5" t="n">
+        <v>161801</v>
+      </c>
+      <c r="C57" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D57" s="5" t="inlineStr">
+        <is>
+          <t>GENERADA</t>
+        </is>
+      </c>
+      <c r="E57" s="5" t="inlineStr">
+        <is>
+          <t>MAURICIO  PARDO MEDINA</t>
+        </is>
+      </c>
+      <c r="F57" s="5" t="inlineStr">
+        <is>
+          <t>79132547</t>
+        </is>
+      </c>
+      <c r="G57" s="5" t="inlineStr">
+        <is>
+          <t>13075-7113</t>
+        </is>
+      </c>
+      <c r="H57" s="5" t="inlineStr">
+        <is>
+          <t>13075-7308</t>
+        </is>
+      </c>
+      <c r="I57" s="5" t="inlineStr">
+        <is>
+          <t>SNC949</t>
+        </is>
+      </c>
+      <c r="J57" s="5" t="inlineStr"/>
+      <c r="K57" s="5" t="inlineStr"/>
+      <c r="L57" s="5" t="inlineStr"/>
+      <c r="M57" s="5" t="inlineStr"/>
+      <c r="N57" s="5" t="inlineStr"/>
+      <c r="O57" s="5" t="inlineStr"/>
+      <c r="P57" s="5" t="inlineStr"/>
+      <c r="Q57" s="5" t="inlineStr"/>
+      <c r="R57" s="5" t="inlineStr"/>
+      <c r="S57" s="5" t="inlineStr"/>
+      <c r="T57" s="5" t="inlineStr"/>
+      <c r="U57" s="10" t="inlineStr"/>
+      <c r="V57" s="10" t="inlineStr"/>
+      <c r="W57" s="10" t="inlineStr"/>
+      <c r="X57" s="10" t="inlineStr"/>
+      <c r="Y57" s="10" t="inlineStr"/>
+      <c r="Z57" s="10" t="inlineStr"/>
+      <c r="AA57" s="10" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="8" t="n">
+        <v>51</v>
+      </c>
+      <c r="B58" s="5" t="n">
+        <v>161802</v>
+      </c>
+      <c r="C58" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D58" s="5" t="inlineStr">
+        <is>
+          <t>GENERADA</t>
+        </is>
+      </c>
+      <c r="E58" s="5" t="inlineStr">
+        <is>
+          <t>MAURICIO  PARDO MEDINA</t>
+        </is>
+      </c>
+      <c r="F58" s="5" t="inlineStr">
+        <is>
+          <t>79132547</t>
+        </is>
+      </c>
+      <c r="G58" s="5" t="inlineStr">
+        <is>
+          <t>13075-7114</t>
+        </is>
+      </c>
+      <c r="H58" s="5" t="inlineStr">
+        <is>
+          <t>13075-7309</t>
+        </is>
+      </c>
+      <c r="I58" s="5" t="inlineStr">
+        <is>
+          <t>SNC949</t>
+        </is>
+      </c>
+      <c r="J58" s="5" t="inlineStr"/>
+      <c r="K58" s="5" t="inlineStr"/>
+      <c r="L58" s="5" t="inlineStr"/>
+      <c r="M58" s="5" t="inlineStr"/>
+      <c r="N58" s="5" t="inlineStr"/>
+      <c r="O58" s="5" t="inlineStr"/>
+      <c r="P58" s="5" t="inlineStr"/>
+      <c r="Q58" s="5" t="inlineStr"/>
+      <c r="R58" s="5" t="inlineStr"/>
+      <c r="S58" s="5" t="inlineStr"/>
+      <c r="T58" s="5" t="inlineStr"/>
+      <c r="U58" s="10" t="inlineStr"/>
+      <c r="V58" s="10" t="inlineStr"/>
+      <c r="W58" s="10" t="inlineStr"/>
+      <c r="X58" s="10" t="inlineStr"/>
+      <c r="Y58" s="10" t="inlineStr"/>
+      <c r="Z58" s="10" t="inlineStr"/>
+      <c r="AA58" s="10" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="8" t="n">
+        <v>52</v>
+      </c>
+      <c r="B59" s="5" t="n">
+        <v>161606</v>
+      </c>
+      <c r="C59" s="9" t="n">
+        <v>44594</v>
+      </c>
+      <c r="D59" s="5" t="inlineStr">
+        <is>
+          <t>FINALIZADA</t>
+        </is>
+      </c>
+      <c r="E59" s="5" t="inlineStr">
+        <is>
+          <t>WILSON LEONIDAS GUTIERREZ BARON</t>
+        </is>
+      </c>
+      <c r="F59" s="5" t="inlineStr">
+        <is>
+          <t>79987585</t>
+        </is>
+      </c>
+      <c r="G59" s="5" t="inlineStr">
+        <is>
+          <t>13075-7091</t>
+        </is>
+      </c>
+      <c r="H59" s="5" t="inlineStr">
+        <is>
+          <t>13075-7290</t>
+        </is>
+      </c>
+      <c r="I59" s="5" t="inlineStr">
+        <is>
+          <t>SMK294</t>
+        </is>
+      </c>
+      <c r="J59" s="11" t="n">
+        <v>44594.94053240741</v>
+      </c>
+      <c r="K59" s="11" t="n">
+        <v>44594.94261574074</v>
+      </c>
+      <c r="L59" s="11" t="n">
+        <v>44594.9571875</v>
+      </c>
+      <c r="M59" s="11" t="n">
+        <v>44594.98070601852</v>
+      </c>
+      <c r="N59" s="11" t="n">
+        <v>44594.9919212963</v>
+      </c>
+      <c r="O59" s="11" t="n">
+        <v>44595.02196759259</v>
+      </c>
+      <c r="P59" s="11" t="n">
+        <v>44595.0303587963</v>
+      </c>
+      <c r="Q59" s="11" t="n">
+        <v>44595.03440972222</v>
+      </c>
+      <c r="R59" s="11" t="n">
+        <v>44595.07375</v>
+      </c>
+      <c r="S59" s="11" t="n">
+        <v>44595.07777777778</v>
+      </c>
+      <c r="T59" s="11" t="n">
+        <v>44595.10164351852</v>
+      </c>
+      <c r="U59" s="10" t="n">
+        <v>0.01665509259259259</v>
+      </c>
+      <c r="V59" s="10" t="n">
+        <v>0.02351851851851852</v>
+      </c>
+      <c r="W59" s="10" t="n">
+        <v>0.01121527777777778</v>
+      </c>
+      <c r="X59" s="10" t="n">
+        <v>0.0300462962962963</v>
+      </c>
+      <c r="Y59" s="10" t="n">
+        <v>0.01244212962962963</v>
+      </c>
+      <c r="Z59" s="10" t="n">
+        <v>0.03934027777777778</v>
+      </c>
+      <c r="AA59" s="10" t="n">
+        <v>0.1611111111111111</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="8" t="n">
+        <v>53</v>
+      </c>
+      <c r="B60" s="5" t="n">
+        <v>161799</v>
+      </c>
+      <c r="C60" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D60" s="5" t="inlineStr">
+        <is>
+          <t>NOTIFICADA</t>
+        </is>
+      </c>
+      <c r="E60" s="5" t="inlineStr">
+        <is>
+          <t>WILSON LEONIDAS GUTIERREZ BARON</t>
+        </is>
+      </c>
+      <c r="F60" s="5" t="inlineStr">
+        <is>
+          <t>79987585</t>
+        </is>
+      </c>
+      <c r="G60" s="5" t="inlineStr">
+        <is>
+          <t>13075-7110</t>
+        </is>
+      </c>
+      <c r="H60" s="5" t="inlineStr">
+        <is>
+          <t>13075-7312</t>
+        </is>
+      </c>
+      <c r="I60" s="5" t="inlineStr">
+        <is>
+          <t>SMK294</t>
+        </is>
+      </c>
+      <c r="J60" s="5" t="inlineStr"/>
+      <c r="K60" s="5" t="inlineStr"/>
+      <c r="L60" s="5" t="inlineStr"/>
+      <c r="M60" s="5" t="inlineStr"/>
+      <c r="N60" s="5" t="inlineStr"/>
+      <c r="O60" s="5" t="inlineStr"/>
+      <c r="P60" s="5" t="inlineStr"/>
+      <c r="Q60" s="5" t="inlineStr"/>
+      <c r="R60" s="5" t="inlineStr"/>
+      <c r="S60" s="5" t="inlineStr"/>
+      <c r="T60" s="5" t="inlineStr"/>
+      <c r="U60" s="10" t="inlineStr"/>
+      <c r="V60" s="10" t="inlineStr"/>
+      <c r="W60" s="10" t="inlineStr"/>
+      <c r="X60" s="10" t="inlineStr"/>
+      <c r="Y60" s="10" t="inlineStr"/>
+      <c r="Z60" s="10" t="inlineStr"/>
+      <c r="AA60" s="10" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="8" t="n">
+        <v>54</v>
+      </c>
+      <c r="B61" s="5" t="n">
+        <v>161800</v>
+      </c>
+      <c r="C61" s="9" t="n">
+        <v>44595</v>
+      </c>
+      <c r="D61" s="5" t="inlineStr">
+        <is>
+          <t>NOTIFICADA</t>
+        </is>
+      </c>
+      <c r="E61" s="5" t="inlineStr">
+        <is>
+          <t>WILSON LEONIDAS GUTIERREZ BARON</t>
+        </is>
+      </c>
+      <c r="F61" s="5" t="inlineStr">
+        <is>
+          <t>79987585</t>
+        </is>
+      </c>
+      <c r="G61" s="5" t="inlineStr">
+        <is>
+          <t>13075-7111</t>
+        </is>
+      </c>
+      <c r="H61" s="5" t="inlineStr">
+        <is>
+          <t>13075-7313</t>
+        </is>
+      </c>
+      <c r="I61" s="5" t="inlineStr">
+        <is>
+          <t>SMK294</t>
+        </is>
+      </c>
+      <c r="J61" s="5" t="inlineStr"/>
+      <c r="K61" s="5" t="inlineStr"/>
+      <c r="L61" s="5" t="inlineStr"/>
+      <c r="M61" s="5" t="inlineStr"/>
+      <c r="N61" s="5" t="inlineStr"/>
+      <c r="O61" s="5" t="inlineStr"/>
+      <c r="P61" s="5" t="inlineStr"/>
+      <c r="Q61" s="5" t="inlineStr"/>
+      <c r="R61" s="5" t="inlineStr"/>
+      <c r="S61" s="5" t="inlineStr"/>
+      <c r="T61" s="5" t="inlineStr"/>
+      <c r="U61" s="10" t="inlineStr"/>
+      <c r="V61" s="10" t="inlineStr"/>
+      <c r="W61" s="10" t="inlineStr"/>
+      <c r="X61" s="10" t="inlineStr"/>
+      <c r="Y61" s="10" t="inlineStr"/>
+      <c r="Z61" s="10" t="inlineStr"/>
+      <c r="AA61" s="10" t="inlineStr"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:Z6"/>

</xml_diff>